<commit_message>
Adding some results, test scripts etc.
</commit_message>
<xml_diff>
--- a/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
+++ b/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
@@ -16,6 +16,62 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>Total loops</t>
+  </si>
+  <si>
+    <t>Loops with API calls</t>
+  </si>
+  <si>
+    <t>Nesting level 1</t>
+  </si>
+  <si>
+    <t>Nesting level 2</t>
+  </si>
+  <si>
+    <t>API calls</t>
+  </si>
+  <si>
+    <t>Loops</t>
+  </si>
+  <si>
+    <t>Methods with different API call count branches</t>
+  </si>
+  <si>
+    <t>Total methods</t>
+  </si>
+  <si>
+    <t>Other methods</t>
+  </si>
+  <si>
+    <t>datastore</t>
+  </si>
+  <si>
+    <t>files</t>
+  </si>
+  <si>
+    <t>taskqueue</t>
+  </si>
+  <si>
+    <t>urlfetch</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>memcache</t>
+  </si>
+  <si>
+    <t>xmpp</t>
+  </si>
+  <si>
+    <t>channel</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -300,11 +356,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2077013160"/>
-        <c:axId val="-2077098984"/>
+        <c:axId val="-2083740392"/>
+        <c:axId val="2127167368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2077013160"/>
+        <c:axId val="-2083740392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -333,12 +389,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077098984"/>
+        <c:crossAx val="2127167368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2077098984"/>
+        <c:axId val="2127167368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -369,7 +425,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077013160"/>
+        <c:crossAx val="-2083740392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -626,11 +682,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2087532040"/>
-        <c:axId val="-2076974328"/>
+        <c:axId val="-2073297784"/>
+        <c:axId val="-2073292328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2087532040"/>
+        <c:axId val="-2073297784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -660,12 +716,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076974328"/>
+        <c:crossAx val="-2073292328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2076974328"/>
+        <c:axId val="-2073292328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -696,9 +752,571 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2087532040"/>
+        <c:crossAx val="-2073297784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Loop</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Nesting Levels</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'30-Apps'!$B$67:$B$68</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Nesting level 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nesting level 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'30-Apps'!$C$67:$C$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>API Calls in Loops CDF</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'30-Apps'!$A$92:$A$99</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'30-Apps'!$C$92:$C$99</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.795180722891566</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.909638554216867</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91566265060241</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.933734939759036</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.94578313253012</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.963855421686747</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.981927710843373</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2083091624"/>
+        <c:axId val="-2080070952"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2083091624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>No. of API calls in a Loop</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2080070952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2080070952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Probability</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2083091624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'30-Apps'!$A$114:$A$115</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Methods with different API call count branches</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Other methods</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'30-Apps'!$B$114:$B$115</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>117.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>791.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>GAE API Calls</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'30-Apps'!$A$138:$A$145</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>datastore</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>files</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>taskqueue</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>urlfetch</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>users</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>memcache</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>xmpp</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>channel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'30-Apps'!$B$138:$B$145</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>643.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2054315304"/>
+        <c:axId val="-2054340120"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2054315304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2054340120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2054340120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2054315304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -772,6 +1390,126 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1102,10 +1840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="O149" sqref="O149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1438,6 +2176,247 @@
       <c r="B29">
         <f>SUM(B1:B27)</f>
         <v>908</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3">
+      <c r="B65" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3">
+      <c r="B66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3">
+      <c r="B67" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3">
+      <c r="B68" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>4</v>
+      </c>
+      <c r="B91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92">
+        <v>0</v>
+      </c>
+      <c r="B92">
+        <v>132</v>
+      </c>
+      <c r="C92">
+        <f>132/166</f>
+        <v>0.79518072289156627</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93">
+        <v>1</v>
+      </c>
+      <c r="B93">
+        <v>19</v>
+      </c>
+      <c r="C93">
+        <f>(B93/166)+C92</f>
+        <v>0.90963855421686746</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94">
+        <v>2</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94">
+        <f t="shared" ref="C94:C99" si="1">(B94/166)+C93</f>
+        <v>0.91566265060240959</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95">
+        <v>3</v>
+      </c>
+      <c r="B95">
+        <v>3</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="1"/>
+        <v>0.9337349397590361</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96">
+        <v>4</v>
+      </c>
+      <c r="B96">
+        <v>2</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="1"/>
+        <v>0.94578313253012047</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97">
+        <v>5</v>
+      </c>
+      <c r="B97">
+        <v>3</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="1"/>
+        <v>0.96385542168674698</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98">
+        <v>7</v>
+      </c>
+      <c r="B98">
+        <v>3</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="1"/>
+        <v>0.98192771084337349</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99">
+        <v>10</v>
+      </c>
+      <c r="B99">
+        <v>3</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="B100">
+        <f>SUM(B92:B99)</f>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>6</v>
+      </c>
+      <c r="B114">
+        <v>117</v>
+      </c>
+      <c r="C114">
+        <f>117/908 *100</f>
+        <v>12.885462555066079</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>8</v>
+      </c>
+      <c r="B115">
+        <f>908-117</f>
+        <v>791</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>7</v>
+      </c>
+      <c r="B116">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
+        <v>9</v>
+      </c>
+      <c r="B138">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" t="s">
+        <v>10</v>
+      </c>
+      <c r="B139">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" t="s">
+        <v>11</v>
+      </c>
+      <c r="B140">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" t="s">
+        <v>12</v>
+      </c>
+      <c r="B141">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" t="s">
+        <v>13</v>
+      </c>
+      <c r="B142">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>14</v>
+      </c>
+      <c r="B143">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>15</v>
+      </c>
+      <c r="B144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" t="s">
+        <v>16</v>
+      </c>
+      <c r="B145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="B146">
+        <f>SUM(B138:B145)</f>
+        <v>726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More results and test scripts
</commit_message>
<xml_diff>
--- a/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
+++ b/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="30-Apps" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Total loops</t>
   </si>
@@ -71,15 +72,49 @@
   <si>
     <t>channel</t>
   </si>
+  <si>
+    <t>Methods with different alloc count branches</t>
+  </si>
+  <si>
+    <t>Methods with no loops</t>
+  </si>
+  <si>
+    <t>Methods with loops</t>
+  </si>
+  <si>
+    <t>API call count</t>
+  </si>
+  <si>
+    <t>Paths</t>
+  </si>
+  <si>
+    <t>Memory allocations</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,13 +137,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -356,11 +395,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2083740392"/>
-        <c:axId val="2127167368"/>
+        <c:axId val="-2051627992"/>
+        <c:axId val="-2051623256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2083740392"/>
+        <c:axId val="-2051627992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -389,12 +428,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127167368"/>
+        <c:crossAx val="-2051623256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2127167368"/>
+        <c:axId val="-2051623256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -425,7 +464,424 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2083740392"/>
+        <c:crossAx val="-2051627992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>No. of Memory Allocations in Paths CDF</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'30-Apps'!$A$209:$A$250</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>92.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>93.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>99.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'30-Apps'!$C$209:$C$250</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>0.170173030623495</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.178048286569313</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.182773440136804</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.185968543977679</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.188713633193079</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.191346218752109</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.193506288954391</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.195013837949733</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.195846365006863</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.197421416196026</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.198298944715703</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.198748959341179</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.20108903539365</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.204441644353442</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.207051729181198</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.208446774520172</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.209549310352586</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.210786850572644</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.256868348221317</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.418153589991675</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.660801476047971</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.862408028260919</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.963211304367392</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.993519789393155</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.998582453929753</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.998942465630133</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.999077470017776</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.999122471480323</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.999167472942871</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.999257475867966</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.999302477330513</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.999347478793061</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.999437481718156</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.999482483180703</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.999572486105798</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.99963998829962</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.999729991224715</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.99981999414981</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.999864995612357</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.999909997074905</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.999954998537452</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2077669944"/>
+        <c:axId val="-2077855992"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2077669944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>No.</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of allocations in Path</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2077855992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2077855992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Probability</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2077669944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -682,11 +1138,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2073297784"/>
-        <c:axId val="-2073292328"/>
+        <c:axId val="-2054361016"/>
+        <c:axId val="-2055076760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2073297784"/>
+        <c:axId val="-2054361016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -716,12 +1172,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073292328"/>
+        <c:crossAx val="-2055076760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2073292328"/>
+        <c:axId val="-2055076760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -752,7 +1208,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073297784"/>
+        <c:crossAx val="-2054361016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -995,11 +1451,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2083091624"/>
-        <c:axId val="-2080070952"/>
+        <c:axId val="-2054357784"/>
+        <c:axId val="-2055055608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2083091624"/>
+        <c:axId val="-2054357784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -1029,12 +1485,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2080070952"/>
+        <c:crossAx val="-2055055608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2080070952"/>
+        <c:axId val="-2055055608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1065,7 +1521,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2083091624"/>
+        <c:crossAx val="-2054357784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1096,7 +1552,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -1282,11 +1738,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2054315304"/>
-        <c:axId val="-2054340120"/>
+        <c:axId val="-2055204552"/>
+        <c:axId val="-2054211736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2054315304"/>
+        <c:axId val="-2055204552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1295,7 +1751,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2054340120"/>
+        <c:crossAx val="-2054211736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1303,7 +1759,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2054340120"/>
+        <c:axId val="-2054211736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1314,9 +1770,440 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2054315304"/>
+        <c:crossAx val="-2055204552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'30-Apps'!$A$118:$A$119</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Methods with different alloc count branches</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Other methods</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'30-Apps'!$B$118:$B$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>749.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'30-Apps'!$A$163:$A$164</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Methods with no loops</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Methods with loops</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'30-Apps'!$B$163:$B$164</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>786.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>122.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>No. of API Calls in Path CDF</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'30-Apps'!$A$186:$A$203</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'30-Apps'!$C$186:$C$203</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.0236257678374547</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.975901716805796</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.979951848435074</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.983844474945436</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.988142114618725</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.991269716265778</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.993294782080418</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.994307314987737</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.995049839119771</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.995544855207794</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.999167472942871</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.999257475867966</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.999617487568346</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.999707490493441</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.999887496343631</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.999909997074905</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.999932497806179</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2084678312"/>
+        <c:axId val="-2084746344"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2084678312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="32.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>No. of GAE API Cals in Path</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2084746344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2084746344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Probability</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2084678312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -1336,13 +2223,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:colOff>660400</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:colOff>635000</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
@@ -1510,6 +2397,126 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>184</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>204</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>208</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>232</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1840,10 +2847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C146"/>
+  <dimension ref="A1:C251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="O149" sqref="O149"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D192" sqref="D192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2349,6 +3356,35 @@
         <v>908</v>
       </c>
     </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>17</v>
+      </c>
+      <c r="B118">
+        <v>159</v>
+      </c>
+      <c r="C118">
+        <f>B118/908 * 100</f>
+        <v>17.51101321585903</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>8</v>
+      </c>
+      <c r="B119">
+        <f>908-159</f>
+        <v>749</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
+        <v>7</v>
+      </c>
+      <c r="B120">
+        <v>908</v>
+      </c>
+    </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
         <v>9</v>
@@ -2419,8 +3455,788 @@
         <v>726</v>
       </c>
     </row>
+    <row r="163" spans="1:3">
+      <c r="A163" t="s">
+        <v>18</v>
+      </c>
+      <c r="B163">
+        <v>786</v>
+      </c>
+      <c r="C163">
+        <f>B163/B165 *100</f>
+        <v>86.563876651982369</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" t="s">
+        <v>19</v>
+      </c>
+      <c r="B164">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" t="s">
+        <v>7</v>
+      </c>
+      <c r="B165">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" t="s">
+        <v>20</v>
+      </c>
+      <c r="B185" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186">
+        <v>0</v>
+      </c>
+      <c r="B186">
+        <v>1050</v>
+      </c>
+      <c r="C186">
+        <f>(B186/B204)</f>
+        <v>2.3625767837454716E-2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187">
+        <v>1</v>
+      </c>
+      <c r="B187">
+        <v>42322</v>
+      </c>
+      <c r="C187">
+        <f>(B187/44443)+C186</f>
+        <v>0.97590171680579618</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188">
+        <v>2</v>
+      </c>
+      <c r="B188">
+        <v>180</v>
+      </c>
+      <c r="C188">
+        <f t="shared" ref="C188:C203" si="2">(B188/44443)+C187</f>
+        <v>0.9799518484350741</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189">
+        <v>3</v>
+      </c>
+      <c r="B189">
+        <v>173</v>
+      </c>
+      <c r="C189">
+        <f t="shared" si="2"/>
+        <v>0.9838444749454357</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190">
+        <v>4</v>
+      </c>
+      <c r="B190">
+        <v>191</v>
+      </c>
+      <c r="C190">
+        <f t="shared" si="2"/>
+        <v>0.98814211461872503</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191">
+        <v>5</v>
+      </c>
+      <c r="B191">
+        <v>139</v>
+      </c>
+      <c r="C191">
+        <f t="shared" si="2"/>
+        <v>0.99126971626577853</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192">
+        <v>6</v>
+      </c>
+      <c r="B192">
+        <v>90</v>
+      </c>
+      <c r="C192">
+        <f t="shared" si="2"/>
+        <v>0.99329478208041755</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193">
+        <v>7</v>
+      </c>
+      <c r="B193">
+        <v>45</v>
+      </c>
+      <c r="C193">
+        <f t="shared" si="2"/>
+        <v>0.99430731498773706</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194">
+        <v>8</v>
+      </c>
+      <c r="B194">
+        <v>33</v>
+      </c>
+      <c r="C194">
+        <f t="shared" si="2"/>
+        <v>0.9950498391197713</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195">
+        <v>9</v>
+      </c>
+      <c r="B195">
+        <v>22</v>
+      </c>
+      <c r="C195">
+        <f t="shared" si="2"/>
+        <v>0.99554485520779412</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196">
+        <v>10</v>
+      </c>
+      <c r="B196">
+        <v>161</v>
+      </c>
+      <c r="C196">
+        <f t="shared" si="2"/>
+        <v>0.99916747294287056</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197">
+        <v>11</v>
+      </c>
+      <c r="B197">
+        <v>4</v>
+      </c>
+      <c r="C197">
+        <f t="shared" si="2"/>
+        <v>0.99925747586796565</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198">
+        <v>12</v>
+      </c>
+      <c r="B198">
+        <v>16</v>
+      </c>
+      <c r="C198">
+        <f t="shared" si="2"/>
+        <v>0.9996174875683459</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199">
+        <v>13</v>
+      </c>
+      <c r="B199">
+        <v>4</v>
+      </c>
+      <c r="C199">
+        <f t="shared" si="2"/>
+        <v>0.99970749049344099</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200">
+        <v>14</v>
+      </c>
+      <c r="B200">
+        <v>8</v>
+      </c>
+      <c r="C200">
+        <f t="shared" si="2"/>
+        <v>0.99988749634363117</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201">
+        <v>27</v>
+      </c>
+      <c r="B201">
+        <v>1</v>
+      </c>
+      <c r="C201">
+        <f t="shared" si="2"/>
+        <v>0.99990999707490491</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202">
+        <v>30</v>
+      </c>
+      <c r="B202">
+        <v>1</v>
+      </c>
+      <c r="C202">
+        <f t="shared" si="2"/>
+        <v>0.99993249780617866</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203">
+        <v>32</v>
+      </c>
+      <c r="B203">
+        <v>3</v>
+      </c>
+      <c r="C203">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="B204">
+        <f>SUM(B186:B203)</f>
+        <v>44443</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208" t="s">
+        <v>22</v>
+      </c>
+      <c r="B208" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209">
+        <v>0</v>
+      </c>
+      <c r="B209">
+        <v>7563</v>
+      </c>
+      <c r="C209">
+        <f>(B209/44443)</f>
+        <v>0.17017303062349526</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210">
+        <v>1</v>
+      </c>
+      <c r="B210">
+        <v>350</v>
+      </c>
+      <c r="C210">
+        <f>(B210/44443)+C209</f>
+        <v>0.17804828656931349</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211">
+        <v>2</v>
+      </c>
+      <c r="B211">
+        <v>210</v>
+      </c>
+      <c r="C211">
+        <f t="shared" ref="C211:C250" si="3">(B211/44443)+C210</f>
+        <v>0.18277344013680444</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212">
+        <v>3</v>
+      </c>
+      <c r="B212">
+        <v>142</v>
+      </c>
+      <c r="C212">
+        <f t="shared" si="3"/>
+        <v>0.18596854397767926</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213">
+        <v>4</v>
+      </c>
+      <c r="B213">
+        <v>122</v>
+      </c>
+      <c r="C213">
+        <f t="shared" si="3"/>
+        <v>0.18871363319307877</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214">
+        <v>5</v>
+      </c>
+      <c r="B214">
+        <v>117</v>
+      </c>
+      <c r="C214">
+        <f t="shared" si="3"/>
+        <v>0.19134621875210944</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215">
+        <v>6</v>
+      </c>
+      <c r="B215">
+        <v>96</v>
+      </c>
+      <c r="C215">
+        <f t="shared" si="3"/>
+        <v>0.19350628895439101</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216">
+        <v>7</v>
+      </c>
+      <c r="B216">
+        <v>67</v>
+      </c>
+      <c r="C216">
+        <f t="shared" si="3"/>
+        <v>0.19501383794973337</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217">
+        <v>8</v>
+      </c>
+      <c r="B217">
+        <v>37</v>
+      </c>
+      <c r="C217">
+        <f t="shared" si="3"/>
+        <v>0.19584636500686273</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218">
+        <v>9</v>
+      </c>
+      <c r="B218">
+        <v>70</v>
+      </c>
+      <c r="C218">
+        <f t="shared" si="3"/>
+        <v>0.19742141619602638</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219">
+        <v>10</v>
+      </c>
+      <c r="B219">
+        <v>39</v>
+      </c>
+      <c r="C219">
+        <f t="shared" si="3"/>
+        <v>0.19829894471570328</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220">
+        <v>11</v>
+      </c>
+      <c r="B220">
+        <v>20</v>
+      </c>
+      <c r="C220">
+        <f t="shared" si="3"/>
+        <v>0.19874895934117862</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221">
+        <v>12</v>
+      </c>
+      <c r="B221">
+        <v>104</v>
+      </c>
+      <c r="C221">
+        <f t="shared" si="3"/>
+        <v>0.20108903539365033</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222">
+        <v>13</v>
+      </c>
+      <c r="B222">
+        <v>149</v>
+      </c>
+      <c r="C222">
+        <f t="shared" si="3"/>
+        <v>0.20444164435344153</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223">
+        <v>14</v>
+      </c>
+      <c r="B223">
+        <v>116</v>
+      </c>
+      <c r="C223">
+        <f t="shared" si="3"/>
+        <v>0.20705172918119844</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224">
+        <v>15</v>
+      </c>
+      <c r="B224">
+        <v>62</v>
+      </c>
+      <c r="C224">
+        <f t="shared" si="3"/>
+        <v>0.20844677452017196</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3">
+      <c r="A225">
+        <v>16</v>
+      </c>
+      <c r="B225">
+        <v>49</v>
+      </c>
+      <c r="C225">
+        <f t="shared" si="3"/>
+        <v>0.2095493103525865</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226">
+        <v>17</v>
+      </c>
+      <c r="B226">
+        <v>55</v>
+      </c>
+      <c r="C226">
+        <f t="shared" si="3"/>
+        <v>0.21078685057264365</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3">
+      <c r="A227">
+        <v>18</v>
+      </c>
+      <c r="B227">
+        <v>2048</v>
+      </c>
+      <c r="C227">
+        <f t="shared" si="3"/>
+        <v>0.25686834822131721</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
+      <c r="A228">
+        <v>19</v>
+      </c>
+      <c r="B228">
+        <v>7168</v>
+      </c>
+      <c r="C228">
+        <f t="shared" si="3"/>
+        <v>0.41815358999167473</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3">
+      <c r="A229">
+        <v>20</v>
+      </c>
+      <c r="B229">
+        <v>10784</v>
+      </c>
+      <c r="C229">
+        <f t="shared" si="3"/>
+        <v>0.66080147604797157</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
+      <c r="A230">
+        <v>21</v>
+      </c>
+      <c r="B230">
+        <v>8960</v>
+      </c>
+      <c r="C230">
+        <f t="shared" si="3"/>
+        <v>0.86240802826091856</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231">
+        <v>22</v>
+      </c>
+      <c r="B231">
+        <v>4480</v>
+      </c>
+      <c r="C231">
+        <f t="shared" si="3"/>
+        <v>0.963211304367392</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232">
+        <v>23</v>
+      </c>
+      <c r="B232">
+        <v>1347</v>
+      </c>
+      <c r="C232">
+        <f t="shared" si="3"/>
+        <v>0.99351978939315533</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233">
+        <v>24</v>
+      </c>
+      <c r="B233">
+        <v>225</v>
+      </c>
+      <c r="C233">
+        <f t="shared" si="3"/>
+        <v>0.99858245392975276</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3">
+      <c r="A234">
+        <v>25</v>
+      </c>
+      <c r="B234">
+        <v>16</v>
+      </c>
+      <c r="C234">
+        <f t="shared" si="3"/>
+        <v>0.998942465630133</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3">
+      <c r="A235">
+        <v>26</v>
+      </c>
+      <c r="B235">
+        <v>6</v>
+      </c>
+      <c r="C235">
+        <f t="shared" si="3"/>
+        <v>0.99907747001777558</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236">
+        <v>27</v>
+      </c>
+      <c r="B236">
+        <v>2</v>
+      </c>
+      <c r="C236">
+        <f t="shared" si="3"/>
+        <v>0.99912247148032307</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3">
+      <c r="A237">
+        <v>33</v>
+      </c>
+      <c r="B237">
+        <v>2</v>
+      </c>
+      <c r="C237">
+        <f t="shared" si="3"/>
+        <v>0.99916747294287056</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
+      <c r="A238">
+        <v>35</v>
+      </c>
+      <c r="B238">
+        <v>4</v>
+      </c>
+      <c r="C238">
+        <f t="shared" si="3"/>
+        <v>0.99925747586796565</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3">
+      <c r="A239">
+        <v>37</v>
+      </c>
+      <c r="B239">
+        <v>2</v>
+      </c>
+      <c r="C239">
+        <f t="shared" si="3"/>
+        <v>0.99930247733051314</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3">
+      <c r="A240">
+        <v>38</v>
+      </c>
+      <c r="B240">
+        <v>2</v>
+      </c>
+      <c r="C240">
+        <f t="shared" si="3"/>
+        <v>0.99934747879306063</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3">
+      <c r="A241">
+        <v>42</v>
+      </c>
+      <c r="B241">
+        <v>4</v>
+      </c>
+      <c r="C241">
+        <f t="shared" si="3"/>
+        <v>0.99943748171815572</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
+      <c r="A242">
+        <v>44</v>
+      </c>
+      <c r="B242">
+        <v>2</v>
+      </c>
+      <c r="C242">
+        <f t="shared" si="3"/>
+        <v>0.99948248318070321</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
+      <c r="A243">
+        <v>53</v>
+      </c>
+      <c r="B243">
+        <v>4</v>
+      </c>
+      <c r="C243">
+        <f t="shared" si="3"/>
+        <v>0.9995724861057983</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3">
+      <c r="A244">
+        <v>54</v>
+      </c>
+      <c r="B244">
+        <v>3</v>
+      </c>
+      <c r="C244">
+        <f t="shared" si="3"/>
+        <v>0.99963998829961964</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3">
+      <c r="A245">
+        <v>90</v>
+      </c>
+      <c r="B245">
+        <v>4</v>
+      </c>
+      <c r="C245">
+        <f t="shared" si="3"/>
+        <v>0.99972999122471473</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3">
+      <c r="A246">
+        <v>91</v>
+      </c>
+      <c r="B246">
+        <v>4</v>
+      </c>
+      <c r="C246">
+        <f t="shared" si="3"/>
+        <v>0.99981999414980982</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
+      <c r="A247">
+        <v>92</v>
+      </c>
+      <c r="B247">
+        <v>2</v>
+      </c>
+      <c r="C247">
+        <f t="shared" si="3"/>
+        <v>0.99986499561235731</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248">
+        <v>93</v>
+      </c>
+      <c r="B248">
+        <v>2</v>
+      </c>
+      <c r="C248">
+        <f t="shared" si="3"/>
+        <v>0.9999099970749048</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3">
+      <c r="A249">
+        <v>99</v>
+      </c>
+      <c r="B249">
+        <v>2</v>
+      </c>
+      <c r="C249">
+        <f t="shared" si="3"/>
+        <v>0.99995499853745229</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3">
+      <c r="A250">
+        <v>100</v>
+      </c>
+      <c r="B250">
+        <v>2</v>
+      </c>
+      <c r="C250">
+        <f t="shared" si="3"/>
+        <v>0.99999999999999978</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3">
+      <c r="B251">
+        <f>SUM(B209:B250)</f>
+        <v>44443</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A209:B250">
+    <sortCondition ref="A209"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -2428,4 +4244,120 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>42322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <f>SUM(A1:A18)</f>
+        <v>44444</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added more GAE signatures to the CFGAnalyzer; Support for detecting user method calls in different packages; data analyzer script; updated results
</commit_message>
<xml_diff>
--- a/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
+++ b/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="28800" windowHeight="15900" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="30-Apps" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="35-Apps" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>Total loops</t>
   </si>
@@ -90,6 +91,18 @@
   <si>
     <t>Memory allocations</t>
   </si>
+  <si>
+    <t>images</t>
+  </si>
+  <si>
+    <t>blobstore</t>
+  </si>
+  <si>
+    <t>tools</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
 </sst>
 </file>
 
@@ -137,17 +150,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -395,11 +428,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2051627992"/>
-        <c:axId val="-2051623256"/>
+        <c:axId val="-2055130776"/>
+        <c:axId val="2083831368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2051627992"/>
+        <c:axId val="-2055130776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -428,12 +461,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2051623256"/>
+        <c:crossAx val="2083831368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2051623256"/>
+        <c:axId val="2083831368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -464,7 +497,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2051627992"/>
+        <c:crossAx val="-2055130776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -806,11 +839,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2077669944"/>
-        <c:axId val="-2077855992"/>
+        <c:axId val="-2084589736"/>
+        <c:axId val="-2080516296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2077669944"/>
+        <c:axId val="-2084589736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -845,12 +878,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077855992"/>
+        <c:crossAx val="-2080516296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2077855992"/>
+        <c:axId val="-2080516296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -881,7 +914,1797 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077669944"/>
+        <c:crossAx val="-2084589736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>No. of Paths Through Methods</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (CDF)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'35-Apps'!$A$1:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>138.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>162.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>166.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>216.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1029.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4378.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6562.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>13127.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34992.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'35-Apps'!$C$1:$C$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>0.652263374485597</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.774348422496571</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.831275720164609</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.882030178326475</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.910836762688614</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.91838134430727</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.922496570644719</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.929355281207133</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.94718792866941</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.968449931412894</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.97599451303155</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.978737997256516</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.979423868312757</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.980109739368998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.98079561042524</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.982853223593964</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.983539094650206</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.984224965706447</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.984910836762688</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.986968449931413</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.987654320987654</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99039780521262</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.991769547325103</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.992455418381344</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.993141289437585</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.993827160493827</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.994513031550068</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.99519890260631</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.996570644718792</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.997256515775034</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.997942386831275</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.998628257887517</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.999314128943758</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'35-Apps'!$A$1:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>138.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>162.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>166.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>216.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1029.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4378.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6562.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>13127.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34992.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'35-Apps'!$C$1:$C$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>0.652263374485597</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.774348422496571</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.831275720164609</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.882030178326475</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.910836762688614</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.91838134430727</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.922496570644719</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.929355281207133</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.94718792866941</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.968449931412894</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.97599451303155</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.978737997256516</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.979423868312757</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.980109739368998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.98079561042524</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.982853223593964</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.983539094650206</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.984224965706447</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.984910836762688</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.986968449931413</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.987654320987654</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99039780521262</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.991769547325103</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.992455418381344</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.993141289437585</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.993827160493827</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.994513031550068</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.99519890260631</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.996570644718792</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.997256515775034</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.997942386831275</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.998628257887517</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.999314128943758</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2078042808"/>
+        <c:axId val="-2073709864"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2078042808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2073709864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2073709864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2078042808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>No. of Paths Through Methods</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (CDF): Cutoff at X = 100</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'35-Apps'!$A$1:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>138.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>162.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>166.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>216.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1029.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4378.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6562.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>13127.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34992.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'35-Apps'!$C$1:$C$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>0.652263374485597</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.774348422496571</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.831275720164609</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.882030178326475</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.910836762688614</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.91838134430727</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.922496570644719</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.929355281207133</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.94718792866941</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.968449931412894</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.97599451303155</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.978737997256516</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.979423868312757</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.980109739368998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.98079561042524</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.982853223593964</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.983539094650206</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.984224965706447</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.984910836762688</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.986968449931413</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.987654320987654</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99039780521262</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.991769547325103</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.992455418381344</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.993141289437585</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.993827160493827</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.994513031550068</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.99519890260631</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.996570644718792</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.997256515775034</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.997942386831275</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.998628257887517</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.999314128943758</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2052748552"/>
+        <c:axId val="-2052745592"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2052748552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2052745592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2052745592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2052748552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Loop Nesting Levels</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'35-Apps'!$A$65:$A$66</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Nesting level 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nesting level 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'35-Apps'!$B$65:$B$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>208.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Methods</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> with Different API Call Count Branches</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'35-Apps'!$A$87:$A$88</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Methods with different API call count branches</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Other methods</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'35-Apps'!$B$87:$B$88</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1300.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>GAE API Calls</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'35-Apps'!$A$109:$A$120</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>images</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>urlfetch</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>memcache</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>blobstore</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>files</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>datastore</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>taskqueue</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>xmpp</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>channel</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>tools</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'35-Apps'!$B$109:$B$120</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>793.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2082753496"/>
+        <c:axId val="-2082717368"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2082753496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2082717368"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2082717368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2082753496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>API Call Counts</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> in Loops</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'35-Apps'!$A$134:$A$142</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'35-Apps'!$C$134:$C$142</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.755555555555555</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.862222222222222</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.888888888888889</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.946666666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.968888888888889</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.973333333333333</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.986666666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2050845960"/>
+        <c:axId val="-2051639336"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2050845960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2051639336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2051639336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2050845960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'35-Apps'!$A$156:$A$157</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Methods with no loops</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Methods with loops</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'35-Apps'!$B$156:$B$157</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1286.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>172.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>API Call Counts in Paths</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (CDF)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'35-Apps'!$A$175:$A$193</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'35-Apps'!$C$175:$C$193</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.323556653288052</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.977832664402593</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.983528866934239</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.987650509416487</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.991031182463723</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.993315838221673</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.994705155912319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.995476999073788</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.996094473602964</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.996511268910157</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.998903982710713</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.999089225069466</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.999475146650201</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.999536894103118</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.999799320778018</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.999922815683853</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.999938252547082</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.999953689410312</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2083720008"/>
+        <c:axId val="-2052135272"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2083720008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2052135272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2052135272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2083720008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1138,11 +2961,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2054361016"/>
-        <c:axId val="-2055076760"/>
+        <c:axId val="2126538920"/>
+        <c:axId val="-2054891048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2054361016"/>
+        <c:axId val="2126538920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1172,12 +2995,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2055076760"/>
+        <c:crossAx val="-2054891048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2055076760"/>
+        <c:axId val="-2054891048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1208,7 +3031,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2054361016"/>
+        <c:crossAx val="2126538920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1451,11 +3274,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2054357784"/>
-        <c:axId val="-2055055608"/>
+        <c:axId val="2122577992"/>
+        <c:axId val="-2055100760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2054357784"/>
+        <c:axId val="2122577992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -1485,12 +3308,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2055055608"/>
+        <c:crossAx val="-2055100760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2055055608"/>
+        <c:axId val="-2055100760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1521,7 +3344,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2054357784"/>
+        <c:crossAx val="2122577992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1738,11 +3561,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2055204552"/>
-        <c:axId val="-2054211736"/>
+        <c:axId val="-2055084184"/>
+        <c:axId val="-2055012536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2055204552"/>
+        <c:axId val="-2055084184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1751,7 +3574,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2054211736"/>
+        <c:crossAx val="-2055012536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1759,7 +3582,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2054211736"/>
+        <c:axId val="-2055012536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1770,7 +3593,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2055204552"/>
+        <c:crossAx val="-2055084184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2130,11 +3953,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2084678312"/>
-        <c:axId val="-2084746344"/>
+        <c:axId val="-2054657928"/>
+        <c:axId val="-2054652440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2084678312"/>
+        <c:axId val="-2054657928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32.0"/>
@@ -2165,12 +3988,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2084746344"/>
+        <c:crossAx val="-2054652440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2084746344"/>
+        <c:axId val="-2054652440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2201,7 +4024,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2084678312"/>
+        <c:crossAx val="-2054657928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2517,6 +4340,253 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>194</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2849,8 +4919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D192" sqref="D192"/>
+    <sheetView topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="A163" sqref="A163:A165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4248,6 +6318,985 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C194"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="O182" sqref="O182"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>951</v>
+      </c>
+      <c r="C1">
+        <f>(B1/1458)</f>
+        <v>0.65226337448559668</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>178</v>
+      </c>
+      <c r="C2">
+        <f>(B2/1458)+C1</f>
+        <v>0.77434842249657065</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>83</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C34" si="0">(B3/1458)+C2</f>
+        <v>0.83127572016460904</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>74</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.88203017832647457</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>42</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.91083676268861447</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.91838134430727014</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0.92249657064471868</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.92935528120713295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.94718792866941004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>31</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.96844993141289426</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0.97599451303154994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0.97873799725651567</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0.97942386831275707</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0.98010973936899848</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0.98079561042523988</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0.98285322359396421</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0.98353909465020561</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0.98422496570644702</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0.98491083676268842</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>30</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0.98696844993141275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>33</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>0.98765432098765416</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>36</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0.99039780521261989</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>56</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0.9917695473251027</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>120</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>0.9924554183813441</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>138</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>0.99314128943758551</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>145</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>0.99382716049382691</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>162</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>0.99451303155006832</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>166</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>0.99519890260630972</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>216</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>0.99657064471879253</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>1029</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>0.99725651577503394</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>4378</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>0.99794238683127534</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>6562</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>0.99862825788751675</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>13127</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>0.99931412894375815</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>34992</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999956</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="B35">
+        <f>SUM(B1:B34)</f>
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>8</v>
+      </c>
+      <c r="B88">
+        <f>1458-158</f>
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>7</v>
+      </c>
+      <c r="B89">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>23</v>
+      </c>
+      <c r="B109">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>12</v>
+      </c>
+      <c r="B110">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>13</v>
+      </c>
+      <c r="B111">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>14</v>
+      </c>
+      <c r="B112">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>24</v>
+      </c>
+      <c r="B113">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>10</v>
+      </c>
+      <c r="B114">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>9</v>
+      </c>
+      <c r="B115">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>11</v>
+      </c>
+      <c r="B116">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>15</v>
+      </c>
+      <c r="B117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>16</v>
+      </c>
+      <c r="B118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>25</v>
+      </c>
+      <c r="B119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>26</v>
+      </c>
+      <c r="B120">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134">
+        <v>0</v>
+      </c>
+      <c r="B134">
+        <v>170</v>
+      </c>
+      <c r="C134">
+        <f>(B134/225)</f>
+        <v>0.75555555555555554</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135">
+        <v>1</v>
+      </c>
+      <c r="B135">
+        <v>24</v>
+      </c>
+      <c r="C135">
+        <f>(B135/225)+C134</f>
+        <v>0.86222222222222222</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136">
+        <v>2</v>
+      </c>
+      <c r="B136">
+        <v>6</v>
+      </c>
+      <c r="C136">
+        <f t="shared" ref="C136:C142" si="1">(B136/225)+C135</f>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137">
+        <v>3</v>
+      </c>
+      <c r="B137">
+        <v>7</v>
+      </c>
+      <c r="C137">
+        <f t="shared" si="1"/>
+        <v>0.91999999999999993</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138">
+        <v>4</v>
+      </c>
+      <c r="B138">
+        <v>6</v>
+      </c>
+      <c r="C138">
+        <f t="shared" si="1"/>
+        <v>0.94666666666666655</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139">
+        <v>5</v>
+      </c>
+      <c r="B139">
+        <v>5</v>
+      </c>
+      <c r="C139">
+        <f t="shared" si="1"/>
+        <v>0.9688888888888888</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140">
+        <v>6</v>
+      </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
+      <c r="C140">
+        <f t="shared" si="1"/>
+        <v>0.97333333333333327</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141">
+        <v>7</v>
+      </c>
+      <c r="B141">
+        <v>3</v>
+      </c>
+      <c r="C141">
+        <f t="shared" si="1"/>
+        <v>0.98666666666666658</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142">
+        <v>10</v>
+      </c>
+      <c r="B142">
+        <v>3</v>
+      </c>
+      <c r="C142">
+        <f t="shared" si="1"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="B143">
+        <f>SUM(B134:B142)</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" t="s">
+        <v>18</v>
+      </c>
+      <c r="B156">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>19</v>
+      </c>
+      <c r="B157">
+        <f>1458-1286</f>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" t="s">
+        <v>7</v>
+      </c>
+      <c r="B158">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175">
+        <v>0</v>
+      </c>
+      <c r="B175">
+        <v>20960</v>
+      </c>
+      <c r="C175">
+        <f>(B175/64780)</f>
+        <v>0.32355665328805189</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176">
+        <v>1</v>
+      </c>
+      <c r="B176">
+        <v>42384</v>
+      </c>
+      <c r="C176">
+        <f>(B176/64780)+C175</f>
+        <v>0.97783266440259342</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177">
+        <v>2</v>
+      </c>
+      <c r="B177">
+        <v>369</v>
+      </c>
+      <c r="C177">
+        <f t="shared" ref="C177:C193" si="2">(B177/64780)+C176</f>
+        <v>0.98352886693423902</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178">
+        <v>3</v>
+      </c>
+      <c r="B178">
+        <v>267</v>
+      </c>
+      <c r="C178">
+        <f t="shared" si="2"/>
+        <v>0.98765050941648658</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179">
+        <v>4</v>
+      </c>
+      <c r="B179">
+        <v>219</v>
+      </c>
+      <c r="C179">
+        <f t="shared" si="2"/>
+        <v>0.99103118246372335</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180">
+        <v>5</v>
+      </c>
+      <c r="B180">
+        <v>148</v>
+      </c>
+      <c r="C180">
+        <f t="shared" si="2"/>
+        <v>0.99331583822167335</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181">
+        <v>6</v>
+      </c>
+      <c r="B181">
+        <v>90</v>
+      </c>
+      <c r="C181">
+        <f t="shared" si="2"/>
+        <v>0.99470515591231856</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182">
+        <v>7</v>
+      </c>
+      <c r="B182">
+        <v>50</v>
+      </c>
+      <c r="C182">
+        <f t="shared" si="2"/>
+        <v>0.99547699907378817</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183">
+        <v>8</v>
+      </c>
+      <c r="B183">
+        <v>40</v>
+      </c>
+      <c r="C183">
+        <f t="shared" si="2"/>
+        <v>0.99609447360296388</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184">
+        <v>9</v>
+      </c>
+      <c r="B184">
+        <v>27</v>
+      </c>
+      <c r="C184">
+        <f t="shared" si="2"/>
+        <v>0.99651126891015751</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185">
+        <v>10</v>
+      </c>
+      <c r="B185">
+        <v>155</v>
+      </c>
+      <c r="C185">
+        <f t="shared" si="2"/>
+        <v>0.99890398271071323</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186">
+        <v>11</v>
+      </c>
+      <c r="B186">
+        <v>12</v>
+      </c>
+      <c r="C186">
+        <f t="shared" si="2"/>
+        <v>0.99908922506946596</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187">
+        <v>12</v>
+      </c>
+      <c r="B187">
+        <v>25</v>
+      </c>
+      <c r="C187">
+        <f t="shared" si="2"/>
+        <v>0.99947514665020076</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188">
+        <v>13</v>
+      </c>
+      <c r="B188">
+        <v>4</v>
+      </c>
+      <c r="C188">
+        <f t="shared" si="2"/>
+        <v>0.9995368941031183</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189">
+        <v>14</v>
+      </c>
+      <c r="B189">
+        <v>17</v>
+      </c>
+      <c r="C189">
+        <f t="shared" si="2"/>
+        <v>0.99979932077801792</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190">
+        <v>16</v>
+      </c>
+      <c r="B190">
+        <v>8</v>
+      </c>
+      <c r="C190">
+        <f t="shared" si="2"/>
+        <v>0.99992281568385311</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191">
+        <v>27</v>
+      </c>
+      <c r="B191">
+        <v>1</v>
+      </c>
+      <c r="C191">
+        <f t="shared" si="2"/>
+        <v>0.99993825254708246</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192">
+        <v>30</v>
+      </c>
+      <c r="B192">
+        <v>1</v>
+      </c>
+      <c r="C192">
+        <f t="shared" si="2"/>
+        <v>0.99995368941031182</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193">
+        <v>32</v>
+      </c>
+      <c r="B193">
+        <v>3</v>
+      </c>
+      <c r="C193">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="B194">
+        <f>SUM(B175:B193)</f>
+        <v>64780</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A175:B193">
+    <sortCondition ref="A175"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
adding appscale benchmarking results
</commit_message>
<xml_diff>
--- a/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
+++ b/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15960" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15960" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="30-Apps" sheetId="1" r:id="rId1"/>
     <sheet name="35-Apps" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="AppScale Benchmarking" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
   <si>
     <t>Total loops</t>
   </si>
@@ -102,6 +102,51 @@
   </si>
   <si>
     <t>search</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>put</t>
+  </si>
+  <si>
+    <t>get</t>
+  </si>
+  <si>
+    <t>asList</t>
+  </si>
+  <si>
+    <t>asIterable</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>jdo.makePersistent</t>
+  </si>
+  <si>
+    <t>jdo.getObjectById</t>
+  </si>
+  <si>
+    <t>jdo.close</t>
+  </si>
+  <si>
+    <t>jdo.execute</t>
+  </si>
+  <si>
+    <t>jdo.closeAll</t>
+  </si>
+  <si>
+    <t>jdo.deletePersistent</t>
+  </si>
+  <si>
+    <t>Mean (ms)</t>
+  </si>
+  <si>
+    <t>Std. Deviation</t>
+  </si>
+  <si>
+    <t>Std. Error</t>
   </si>
 </sst>
 </file>
@@ -428,11 +473,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2062087992"/>
-        <c:axId val="-2062081192"/>
+        <c:axId val="-2132713656"/>
+        <c:axId val="-2132012680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2062087992"/>
+        <c:axId val="-2132713656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -461,12 +506,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062081192"/>
+        <c:crossAx val="-2132012680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2062081192"/>
+        <c:axId val="-2132012680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -497,7 +542,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062087992"/>
+        <c:crossAx val="-2132713656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -838,11 +883,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2061804072"/>
-        <c:axId val="-2061798376"/>
+        <c:axId val="-2101248536"/>
+        <c:axId val="-2101334296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2061804072"/>
+        <c:axId val="-2101248536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -876,12 +921,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061798376"/>
+        <c:crossAx val="-2101334296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2061798376"/>
+        <c:axId val="-2101334296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -911,7 +956,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061804072"/>
+        <c:crossAx val="-2101248536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1440,11 +1485,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2061744152"/>
-        <c:axId val="-2061741160"/>
+        <c:axId val="-2130451048"/>
+        <c:axId val="-2101332760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2061744152"/>
+        <c:axId val="-2130451048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1454,12 +1499,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061741160"/>
+        <c:crossAx val="-2101332760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2061741160"/>
+        <c:axId val="-2101332760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1471,7 +1516,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061744152"/>
+        <c:crossAx val="-2130451048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1770,11 +1815,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2061714616"/>
-        <c:axId val="-2061711656"/>
+        <c:axId val="-2126773080"/>
+        <c:axId val="-2128051480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2061714616"/>
+        <c:axId val="-2126773080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1785,12 +1830,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061711656"/>
+        <c:crossAx val="-2128051480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2061711656"/>
+        <c:axId val="-2128051480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1802,7 +1847,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061714616"/>
+        <c:crossAx val="-2126773080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1849,7 +1894,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1904,7 +1948,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1954,7 +1997,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2009,7 +2051,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2054,7 +2095,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2167,11 +2207,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2061639032"/>
-        <c:axId val="-2061636024"/>
+        <c:axId val="-2128070312"/>
+        <c:axId val="-2127257032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2061639032"/>
+        <c:axId val="-2128070312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2180,7 +2220,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061636024"/>
+        <c:crossAx val="-2127257032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2188,7 +2228,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2061636024"/>
+        <c:axId val="-2127257032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2199,7 +2239,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061639032"/>
+        <c:crossAx val="-2128070312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2251,7 +2291,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2348,11 +2387,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2061609976"/>
-        <c:axId val="-2061607016"/>
+        <c:axId val="-2130414488"/>
+        <c:axId val="-2127283592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2061609976"/>
+        <c:axId val="-2130414488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -2363,12 +2402,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061607016"/>
+        <c:crossAx val="-2127283592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2061607016"/>
+        <c:axId val="-2127283592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2380,7 +2419,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061609976"/>
+        <c:crossAx val="-2130414488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2463,7 +2502,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2513,7 +2551,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2670,11 +2707,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2061560072"/>
-        <c:axId val="-2061557112"/>
+        <c:axId val="-2127079560"/>
+        <c:axId val="-2127864984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2061560072"/>
+        <c:axId val="-2127079560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2684,12 +2721,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061557112"/>
+        <c:crossAx val="-2127864984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2061557112"/>
+        <c:axId val="-2127864984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2701,9 +2738,314 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061560072"/>
+        <c:crossAx val="-2127079560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Datastore Average Performance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'AppScale Benchmarking'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'AppScale Benchmarking'!$D$2:$D$12</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>0.138312338677006</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0915412364991755</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.263381276801706</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.00999999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.55912232429539</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.321264861307786</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.0989388138643722</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.0399368187885502</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.187689298382386</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.0</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>1.87186613524654</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'AppScale Benchmarking'!$D$2:$D$12</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>0.138312338677006</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0915412364991755</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.263381276801706</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.00999999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.55912232429539</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.321264861307786</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.0989388138643722</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.0399368187885502</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.187689298382386</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.0</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>1.87186613524654</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'AppScale Benchmarking'!$A$2:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>put</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>get</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>asList</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>asIterable</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>delete</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>jdo.makePersistent</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>jdo.getObjectById</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>jdo.close</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>jdo.execute</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>jdo.closeAll</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>jdo.deletePersistent</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'AppScale Benchmarking'!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>14.81</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54.28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.39</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.03</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.15</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46.34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2127852392"/>
+        <c:axId val="-2128529656"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2127852392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2128529656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2128529656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average Execution Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2127852392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -2957,11 +3299,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2062020184"/>
-        <c:axId val="-2062014728"/>
+        <c:axId val="-2126752408"/>
+        <c:axId val="-2127121080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2062020184"/>
+        <c:axId val="-2126752408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -2990,12 +3332,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062014728"/>
+        <c:crossAx val="-2127121080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2062014728"/>
+        <c:axId val="-2127121080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3025,7 +3367,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062020184"/>
+        <c:crossAx val="-2126752408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3265,11 +3607,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2061963992"/>
-        <c:axId val="-2061958504"/>
+        <c:axId val="-2127979096"/>
+        <c:axId val="-2127636024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2061963992"/>
+        <c:axId val="-2127979096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -3298,12 +3640,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061958504"/>
+        <c:crossAx val="-2127636024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2061958504"/>
+        <c:axId val="-2127636024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3333,7 +3675,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061963992"/>
+        <c:crossAx val="-2127979096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3548,11 +3890,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2061911160"/>
-        <c:axId val="-2061908216"/>
+        <c:axId val="-2126741672"/>
+        <c:axId val="-2127137256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2061911160"/>
+        <c:axId val="-2126741672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3561,7 +3903,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061908216"/>
+        <c:crossAx val="-2127137256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3569,7 +3911,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2061908216"/>
+        <c:axId val="-2127137256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3580,7 +3922,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061911160"/>
+        <c:crossAx val="-2126741672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3937,11 +4279,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2061838824"/>
-        <c:axId val="-2061833336"/>
+        <c:axId val="-2100323640"/>
+        <c:axId val="-2101099912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2061838824"/>
+        <c:axId val="-2100323640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32.0"/>
@@ -3971,12 +4313,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061833336"/>
+        <c:crossAx val="-2101099912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2061833336"/>
+        <c:axId val="-2101099912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4006,7 +4348,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061838824"/>
+        <c:crossAx val="-2100323640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4577,6 +4919,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6302,7 +6679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C194"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C193" sqref="C193"/>
     </sheetView>
   </sheetViews>
@@ -7278,112 +7655,196 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6">
-        <v>42322</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>14.81</v>
+      </c>
+      <c r="C2">
+        <v>1.3831233867700601</v>
+      </c>
+      <c r="D2">
+        <f>(C2/SQRT(100))</f>
+        <v>0.13831233867700601</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="C3">
+        <v>0.91541236499175505</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D12" si="0">(C3/SQRT(100))</f>
+        <v>9.1541236499175505E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>1.18</v>
+      </c>
+      <c r="C4">
+        <v>2.63381276801706</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.26338127680170598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>0.01</v>
+      </c>
+      <c r="C5">
+        <v>9.9999999999999895E-2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999898E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>54.28</v>
+      </c>
+      <c r="C6">
+        <v>25.591223242953902</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>2.55912232429539</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19">
-        <f>SUM(A1:A18)</f>
-        <v>44444</v>
+      <c r="B7">
+        <v>15.39</v>
+      </c>
+      <c r="C7">
+        <v>3.2126486130778602</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.32126486130778603</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>5.03</v>
+      </c>
+      <c r="C8">
+        <v>0.98938813864372199</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>9.8938813864372199E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>0.11</v>
+      </c>
+      <c r="C9">
+        <v>0.39936818788550199</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>3.9936818788550196E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C10">
+        <v>1.8768929838238599</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.18768929838238599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12">
+        <v>46.34</v>
+      </c>
+      <c r="C12">
+        <v>18.7186613524654</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1.87186613524654</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added figure for proposal
</commit_message>
<xml_diff>
--- a/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
+++ b/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15960" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15960" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="30-Apps" sheetId="1" r:id="rId1"/>
     <sheet name="35-Apps" sheetId="3" r:id="rId2"/>
-    <sheet name="AppScale Benchmarking" sheetId="2" r:id="rId3"/>
-    <sheet name="Predictions" sheetId="4" r:id="rId4"/>
-    <sheet name="Predictions-Raw" sheetId="5" r:id="rId5"/>
+    <sheet name="pred-meas.g" sheetId="7" r:id="rId3"/>
+    <sheet name="pred-meas" sheetId="6" r:id="rId4"/>
+    <sheet name="AppScale Benchmarking" sheetId="2" r:id="rId5"/>
+    <sheet name="Predictions" sheetId="4" r:id="rId6"/>
+    <sheet name="Predictions-Raw" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="130406" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="51">
   <si>
     <t>Total loops</t>
   </si>
@@ -181,8 +183,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -214,6 +222,10 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -232,20 +244,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -253,41 +253,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -310,14 +289,11 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -504,25 +480,16 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="2043637256"/>
-        <c:axId val="2042627640"/>
+        <c:dLbls/>
+        <c:axId val="634793656"/>
+        <c:axId val="634760056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2043637256"/>
+        <c:axId val="634793656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -540,23 +507,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2042627640"/>
+        <c:crossAx val="634760056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2042627640"/>
+        <c:axId val="634760056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -575,20 +538,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2043637256"/>
+        <c:crossAx val="634793656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -600,17 +559,8 @@
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -628,14 +578,11 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -912,26 +859,17 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-2091987544"/>
-        <c:axId val="-2091981848"/>
+        <c:dLbls/>
+        <c:axId val="635187176"/>
+        <c:axId val="635182552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2091987544"/>
+        <c:axId val="635187176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -954,23 +892,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2091981848"/>
+        <c:crossAx val="635182552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2091981848"/>
+        <c:axId val="635182552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -989,20 +923,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2091987544"/>
+        <c:crossAx val="635187176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1014,17 +944,8 @@
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1047,14 +968,11 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="1"/>
@@ -1283,7 +1201,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1513,55 +1430,40 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-2091931240"/>
-        <c:axId val="-2091928248"/>
+        <c:dLbls/>
+        <c:axId val="635230360"/>
+        <c:axId val="635252344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2091931240"/>
+        <c:axId val="635230360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2091928248"/>
+        <c:crossAx val="635252344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2091928248"/>
+        <c:axId val="635252344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2091931240"/>
+        <c:crossAx val="635230360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1573,17 +1475,8 @@
 
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1606,14 +1499,11 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -1842,56 +1732,41 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-2092889528"/>
-        <c:axId val="-2092892488"/>
+        <c:dLbls/>
+        <c:axId val="635272552"/>
+        <c:axId val="635275752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2092889528"/>
+        <c:axId val="635272552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092892488"/>
+        <c:crossAx val="635275752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2092892488"/>
+        <c:axId val="635275752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092889528"/>
+        <c:crossAx val="635272552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1903,17 +1778,8 @@
 
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1931,9 +1797,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -1971,25 +1835,15 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2001,17 +1855,8 @@
 
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2034,9 +1879,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -2074,25 +1917,15 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2104,17 +1937,8 @@
 
 <file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2132,19 +1956,15 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'35-Apps'!$A$109:$A$120</c:f>
@@ -2235,55 +2055,39 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-2092950872"/>
-        <c:axId val="2135926872"/>
+        <c:dLbls/>
+        <c:axId val="635363384"/>
+        <c:axId val="635354360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2092950872"/>
+        <c:axId val="635363384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135926872"/>
+        <c:crossAx val="635354360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2135926872"/>
+        <c:axId val="635354360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092950872"/>
+        <c:crossAx val="635363384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2295,17 +2099,8 @@
 
 <file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2328,14 +2123,11 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -2414,56 +2206,41 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="2135805272"/>
-        <c:axId val="2135808232"/>
+        <c:dLbls/>
+        <c:axId val="635389656"/>
+        <c:axId val="635392872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2135805272"/>
+        <c:axId val="635389656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135808232"/>
+        <c:crossAx val="635392872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2135808232"/>
+        <c:axId val="635392872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135805272"/>
+        <c:crossAx val="635389656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2475,19 +2252,9 @@
 
 <file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -2525,25 +2292,15 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2555,17 +2312,8 @@
 
 <file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2588,14 +2336,11 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -2734,55 +2479,40 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="2135743576"/>
-        <c:axId val="2135746536"/>
+        <c:dLbls/>
+        <c:axId val="634581912"/>
+        <c:axId val="634577560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2135743576"/>
+        <c:axId val="634581912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135746536"/>
+        <c:crossAx val="634577560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2135746536"/>
+        <c:axId val="634577560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135743576"/>
+        <c:crossAx val="634581912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2794,17 +2524,534 @@
 
 <file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>Predictions</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" baseline="0"/>
+              <a:t> and Measurements</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>"mean measurement"</c:v>
+          </c:tx>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Predictions-Raw'!$I$82:$I$85</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>12.02144548359943</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6.35565444579412</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.530973081584815</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Predictions-Raw'!$J$82:$J$85</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>12.02144548359943</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6.35565444579412</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.530973081584815</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Predictions-Raw'!$G$82:$G$84</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ServerHealth#info</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DateEngine#browse</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>App-Engine-Mapper#addComment</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Predictions-Raw'!$H$82:$H$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>23.34999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.22999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>prediction</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Predictions-Raw'!$G$82:$G$84</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ServerHealth#info</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DateEngine#browse</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>App-Engine-Mapper#addComment</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Predictions!$C$9:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>13.44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="797407400"/>
+        <c:axId val="797152520"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="797407400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="797152520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="797152520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Average Execution Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="797407400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>No. of Paths</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Through Method (CDF) - Cutoff at x = 100</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'30-Apps'!$A$1:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>138.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>162.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>216.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6562.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>34992.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'30-Apps'!$C$1:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.677312775330396</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.822687224669603</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.875550660792951</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.898678414096916</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.919603524229075</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.927312775330396</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.932819383259912</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.941629955947136</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.95704845814978</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.963656387665198</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.975770925110132</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.977973568281938</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.979074889867841</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.980176211453744</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.983480176211454</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.984581497797357</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.98568281938326</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.986784140969163</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.987885462555066</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.988986784140969</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.992290748898678</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.993392070484581</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.994493392070484</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.995594713656387</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.997797356828193</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.998898678414096</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.999999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:dLbls/>
+        <c:axId val="634930872"/>
+        <c:axId val="634948936"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="634930872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100.0"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>No. of Paths</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="634948936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634948936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Probability</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="634930872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2822,15 +3069,13 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2845,11 +3090,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'AppScale Benchmarking'!$D$2:$D$12</c:f>
@@ -3019,41 +3262,28 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-2094910296"/>
-        <c:axId val="-2120383368"/>
+        <c:dLbls/>
+        <c:axId val="634523592"/>
+        <c:axId val="634538936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2094910296"/>
+        <c:axId val="634523592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120383368"/>
+        <c:crossAx val="634538936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2120383368"/>
+        <c:axId val="634538936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -3072,344 +3302,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094910296"/>
+        <c:crossAx val="634523592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>No. of Paths</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Through Method (CDF) - Cutoff at x = 100</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'30-Apps'!$A$1:$A$27</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>25.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>30.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>33.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>36.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>138.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>145.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>162.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>216.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>6562.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>34992.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'30-Apps'!$C$1:$C$27</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>0.677312775330396</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.822687224669603</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.875550660792951</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.898678414096916</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.919603524229075</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.927312775330396</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.932819383259912</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.941629955947136</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.95704845814978</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.963656387665198</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.975770925110132</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.977973568281938</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.979074889867841</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.980176211453744</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.983480176211454</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.984581497797357</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.98568281938326</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.986784140969163</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.987885462555066</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.988986784140969</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.992290748898678</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.993392070484581</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.994493392070484</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.995594713656387</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.997797356828193</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.998898678414096</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.999999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="2120071992"/>
-        <c:axId val="2119277560"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="2120071992"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="100.0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>No. of Paths</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2119277560"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="2119277560"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Probability</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120071992"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3421,17 +3324,8 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3454,9 +3348,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -3494,25 +3386,15 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3524,17 +3406,8 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3552,14 +3425,11 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -3632,26 +3502,17 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-2096855048"/>
-        <c:axId val="-2096841176"/>
+        <c:dLbls/>
+        <c:axId val="634998040"/>
+        <c:axId val="635009336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2096855048"/>
+        <c:axId val="634998040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -3669,23 +3530,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2096841176"/>
+        <c:crossAx val="635009336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2096841176"/>
+        <c:axId val="635009336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -3704,20 +3561,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2096855048"/>
+        <c:crossAx val="634998040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3729,17 +3582,8 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -3779,25 +3623,15 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3809,17 +3643,8 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3837,19 +3662,15 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'30-Apps'!$A$138:$A$145</c:f>
@@ -3916,55 +3737,39 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-2096859608"/>
-        <c:axId val="-2096856664"/>
+        <c:dLbls/>
+        <c:axId val="635062952"/>
+        <c:axId val="635053912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2096859608"/>
+        <c:axId val="635062952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2096856664"/>
+        <c:crossAx val="635053912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2096856664"/>
+        <c:axId val="635053912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2096859608"/>
+        <c:crossAx val="635062952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3976,19 +3781,9 @@
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -4026,25 +3821,15 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4056,19 +3841,9 @@
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -4106,25 +3881,15 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4136,17 +3901,8 @@
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -4164,14 +3920,11 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -4304,27 +4057,18 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-2092027400"/>
-        <c:axId val="-2092021896"/>
+        <c:dLbls/>
+        <c:axId val="635140200"/>
+        <c:axId val="635147816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2092027400"/>
+        <c:axId val="635140200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32.0"/>
           <c:min val="0.0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -4342,23 +4086,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092021896"/>
+        <c:crossAx val="635147816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2092021896"/>
+        <c:axId val="635147816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -4377,20 +4117,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092027400"/>
+        <c:crossAx val="635140200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4398,6 +4134,17 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr published="0"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4956,6 +4703,33 @@
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8570280" cy="5826014"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
@@ -5310,14 +5084,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C251"/>
   <sheetViews>
     <sheetView topLeftCell="A222" workbookViewId="0">
       <selection activeCell="A163" sqref="A163:A165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1">
@@ -6697,13 +6472,13 @@
     </row>
   </sheetData>
   <sortState ref="A209:B250">
-    <sortCondition ref="A209"/>
+    <sortCondition ref="A209:A250"/>
   </sortState>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -6711,14 +6486,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C193" sqref="C193"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1">
@@ -7675,13 +7451,14 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A175:B193">
-    <sortCondition ref="A175"/>
+    <sortCondition ref="A175:A193"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -7689,14 +7466,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -7883,11 +7661,10 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -7895,14 +7672,222 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>14.81</v>
+      </c>
+      <c r="C2">
+        <v>1.3831233867700601</v>
+      </c>
+      <c r="D2">
+        <f>(C2/SQRT(100))</f>
+        <v>0.13831233867700601</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="C3">
+        <v>0.91541236499175505</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D12" si="0">(C3/SQRT(100))</f>
+        <v>9.1541236499175505E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>1.18</v>
+      </c>
+      <c r="C4">
+        <v>2.63381276801706</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.26338127680170598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>0.01</v>
+      </c>
+      <c r="C5">
+        <v>9.9999999999999895E-2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999898E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>54.28</v>
+      </c>
+      <c r="C6">
+        <v>25.591223242953902</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>2.55912232429539</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>15.39</v>
+      </c>
+      <c r="C7">
+        <v>3.2126486130778602</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.32126486130778603</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>5.03</v>
+      </c>
+      <c r="C8">
+        <v>0.98938813864372199</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>9.8938813864372199E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>0.11</v>
+      </c>
+      <c r="C9">
+        <v>0.39936818788550199</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>3.9936818788550196E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C10">
+        <v>1.8768929838238599</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.18768929838238599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12">
+        <v>46.34</v>
+      </c>
+      <c r="C12">
+        <v>18.7186613524654</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1.87186613524654</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
   </cols>
@@ -7983,25 +7968,44 @@
         <v>6.42</v>
       </c>
     </row>
+    <row r="9" spans="1:4">
+      <c r="C9">
+        <f>4.48*3</f>
+        <v>13.440000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="C10">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="C11">
+        <v>14.81</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D103"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103:D103"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="J85" sqref="J85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -9123,7 +9127,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:10">
       <c r="A81">
         <v>2.3E-2</v>
       </c>
@@ -9137,7 +9141,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:10">
       <c r="A82">
         <v>2.8000000000000001E-2</v>
       </c>
@@ -9150,8 +9154,23 @@
       <c r="D82">
         <v>1.9E-2</v>
       </c>
-    </row>
-    <row r="83" spans="1:4">
+      <c r="G82" t="s">
+        <v>44</v>
+      </c>
+      <c r="H82">
+        <f>$A103</f>
+        <v>23.349999999999984</v>
+      </c>
+      <c r="I82">
+        <f>A104*2</f>
+        <v>12.021445483599427</v>
+      </c>
+      <c r="J82">
+        <f>A104*2</f>
+        <v>12.021445483599427</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -9164,8 +9183,23 @@
       <c r="D83">
         <v>2.1000000000000001E-2</v>
       </c>
-    </row>
-    <row r="84" spans="1:4">
+      <c r="G83" t="s">
+        <v>48</v>
+      </c>
+      <c r="H83">
+        <f>$C103</f>
+        <v>10.320000000000004</v>
+      </c>
+      <c r="I83">
+        <f>C104*2</f>
+        <v>6.3556544457941193</v>
+      </c>
+      <c r="J83">
+        <f>C104*2</f>
+        <v>6.3556544457941193</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84">
         <v>2.1000000000000001E-2</v>
       </c>
@@ -9178,8 +9212,23 @@
       <c r="D84">
         <v>1.9E-2</v>
       </c>
-    </row>
-    <row r="85" spans="1:4">
+      <c r="G84" t="s">
+        <v>49</v>
+      </c>
+      <c r="H84">
+        <f>D103</f>
+        <v>21.229999999999993</v>
+      </c>
+      <c r="I84">
+        <f>D104*2</f>
+        <v>7.5309730815848157</v>
+      </c>
+      <c r="J84">
+        <f>D104*2</f>
+        <v>7.5309730815848157</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85">
         <v>2.1000000000000001E-2</v>
       </c>
@@ -9193,7 +9242,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:10">
       <c r="A86">
         <v>2.1000000000000001E-2</v>
       </c>
@@ -9207,7 +9256,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:10">
       <c r="A87">
         <v>2.1000000000000001E-2</v>
       </c>
@@ -9221,7 +9270,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:10">
       <c r="A88">
         <v>0.02</v>
       </c>
@@ -9235,7 +9284,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:10">
       <c r="A89">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -9249,7 +9298,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:10">
       <c r="A90">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -9263,7 +9312,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:10">
       <c r="A91">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -9277,7 +9326,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:10">
       <c r="A92">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -9291,7 +9340,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:10">
       <c r="A93">
         <v>2.3E-2</v>
       </c>
@@ -9305,7 +9354,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:10">
       <c r="A94">
         <v>2.3E-2</v>
       </c>
@@ -9319,7 +9368,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:10">
       <c r="A95">
         <v>2.3E-2</v>
       </c>
@@ -9333,7 +9382,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:10">
       <c r="A96">
         <v>2.3E-2</v>
       </c>
@@ -9435,10 +9484,31 @@
         <v>21.229999999999993</v>
       </c>
     </row>
+    <row r="104" spans="1:4">
+      <c r="A104">
+        <f>STDEV(A2:A101)*1000</f>
+        <v>6.0107227417997136</v>
+      </c>
+      <c r="B104">
+        <f>STDEV(B2:B101)*1000</f>
+        <v>193.80373572198766</v>
+      </c>
+      <c r="C104">
+        <f>STDEV(C2:C101)*1000</f>
+        <v>3.1778272228970597</v>
+      </c>
+      <c r="D104">
+        <f>STDEV(D2:D101)*1000</f>
+        <v>3.7654865407924079</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
adding latest results and test scripts
</commit_message>
<xml_diff>
--- a/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
+++ b/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15960" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16080" tabRatio="500" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="30-Apps" sheetId="1" r:id="rId1"/>
@@ -14,10 +14,11 @@
     <sheet name="AppScale Benchmarking" sheetId="2" r:id="rId5"/>
     <sheet name="Predictions" sheetId="4" r:id="rId6"/>
     <sheet name="Predictions-Raw" sheetId="5" r:id="rId7"/>
+    <sheet name="Kitty" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="130406" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="59">
   <si>
     <t>Total loops</t>
   </si>
@@ -179,18 +180,36 @@
   <si>
     <t>Offset</t>
   </si>
+  <si>
+    <t>Predicted Quantile</t>
+  </si>
+  <si>
+    <t>Actual Quantile</t>
+  </si>
+  <si>
+    <t>Actual Quantile (QBETS)</t>
+  </si>
+  <si>
+    <t>51ms/1123</t>
+  </si>
+  <si>
+    <t>41ms/100</t>
+  </si>
+  <si>
+    <t>44ms/100</t>
+  </si>
+  <si>
+    <t>43ms/1123</t>
+  </si>
+  <si>
+    <t>44ms/1123</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -244,29 +263,47 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -289,11 +326,15 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -480,16 +521,25 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="634793656"/>
-        <c:axId val="634760056"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2128263304"/>
+        <c:axId val="-2128257896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="634793656"/>
+        <c:axId val="-2128263304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -507,19 +557,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="634760056"/>
+        <c:crossAx val="-2128257896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="634760056"/>
+        <c:axId val="-2128257896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -538,16 +593,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="634793656"/>
+        <c:crossAx val="-2128263304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -559,8 +619,17 @@
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -578,11 +647,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -859,17 +931,26 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="635187176"/>
-        <c:axId val="635182552"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2127959960"/>
+        <c:axId val="-2127954152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="635187176"/>
+        <c:axId val="-2127959960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -892,19 +973,23 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="635182552"/>
+        <c:crossAx val="-2127954152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="635182552"/>
+        <c:axId val="-2127954152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -923,16 +1008,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="635187176"/>
+        <c:crossAx val="-2127959960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -944,8 +1033,17 @@
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -968,11 +1066,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="1"/>
@@ -1201,6 +1302,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1430,40 +1532,55 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="635230360"/>
-        <c:axId val="635252344"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2129990696"/>
+        <c:axId val="-2129987704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="635230360"/>
+        <c:axId val="-2129990696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="635252344"/>
+        <c:crossAx val="-2129987704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="635252344"/>
+        <c:axId val="-2129987704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="635230360"/>
+        <c:crossAx val="-2129990696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1475,8 +1592,17 @@
 
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1499,11 +1625,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -1732,41 +1861,56 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="635272552"/>
-        <c:axId val="635275752"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2129958600"/>
+        <c:axId val="-2129955608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="635272552"/>
+        <c:axId val="-2129958600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="635275752"/>
+        <c:crossAx val="-2129955608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="635275752"/>
+        <c:axId val="-2129955608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="635272552"/>
+        <c:crossAx val="-2129958600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1778,8 +1922,17 @@
 
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1797,7 +1950,9 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -1835,15 +1990,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1855,8 +2020,17 @@
 
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1879,7 +2053,9 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -1917,15 +2093,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1937,8 +2123,17 @@
 
 <file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1956,15 +2151,19 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'35-Apps'!$A$109:$A$120</c:f>
@@ -2055,39 +2254,55 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="635363384"/>
-        <c:axId val="635354360"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2129877128"/>
+        <c:axId val="-2129874152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="635363384"/>
+        <c:axId val="-2129877128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="635354360"/>
+        <c:crossAx val="-2129874152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="635354360"/>
+        <c:axId val="-2129874152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="635363384"/>
+        <c:crossAx val="-2129877128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2099,8 +2314,17 @@
 
 <file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2123,11 +2347,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -2206,41 +2433,56 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="635389656"/>
-        <c:axId val="635392872"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2129846472"/>
+        <c:axId val="-2129843480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="635389656"/>
+        <c:axId val="-2129846472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="635392872"/>
+        <c:crossAx val="-2129843480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="635392872"/>
+        <c:axId val="-2129843480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="635389656"/>
+        <c:crossAx val="-2129846472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2252,9 +2494,19 @@
 
 <file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -2292,15 +2544,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2312,8 +2574,17 @@
 
 <file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2336,11 +2607,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -2479,40 +2753,55 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="634581912"/>
-        <c:axId val="634577560"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2129793128"/>
+        <c:axId val="-2129790136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="634581912"/>
+        <c:axId val="-2129793128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="634577560"/>
+        <c:crossAx val="-2129790136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="634577560"/>
+        <c:axId val="-2129790136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="634581912"/>
+        <c:crossAx val="-2129793128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2524,8 +2813,17 @@
 
 <file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2549,21 +2847,26 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>"mean measurement"</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Predictions-Raw'!$I$82:$I$85</c:f>
@@ -2574,10 +2877,10 @@
                     <c:v>12.02144548359943</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>6.35565444579412</c:v>
+                    <c:v>6.35565444579419</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.530973081584815</c:v>
+                    <c:v>7.530973081584847</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2592,10 +2895,10 @@
                     <c:v>12.02144548359943</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>6.35565444579412</c:v>
+                    <c:v>6.35565444579419</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.530973081584815</c:v>
+                    <c:v>7.530973081584847</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2643,6 +2946,7 @@
           <c:tx>
             <c:v>prediction</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Predictions-Raw'!$G$82:$G$84</c:f>
@@ -2679,15 +2983,27 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="797407400"/>
-        <c:axId val="797152520"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2129740424"/>
+        <c:axId val="-2129737416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="797407400"/>
+        <c:axId val="-2129740424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2699,17 +3015,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="797152520"/>
+        <c:crossAx val="-2129737416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="797152520"/>
+        <c:axId val="-2129737416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -2729,8 +3047,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2742,21 +3063,31 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="797407400"/>
+        <c:crossAx val="-2129740424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2779,11 +3110,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -2970,17 +3304,26 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="634930872"/>
-        <c:axId val="634948936"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2128189640"/>
+        <c:axId val="-2128184120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="634930872"/>
+        <c:axId val="-2128189640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2998,19 +3341,23 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="634948936"/>
+        <c:crossAx val="-2128184120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="634948936"/>
+        <c:axId val="-2128184120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -3029,16 +3376,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="634930872"/>
+        <c:crossAx val="-2128189640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3050,8 +3401,17 @@
 
 <file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3069,13 +3429,15 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -3090,9 +3452,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'AppScale Benchmarking'!$D$2:$D$12</c:f>
@@ -3262,28 +3626,41 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="634523592"/>
-        <c:axId val="634538936"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2136706712"/>
+        <c:axId val="2136709688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="634523592"/>
+        <c:axId val="2136706712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="634538936"/>
+        <c:crossAx val="2136709688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="634538936"/>
+        <c:axId val="2136709688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -3302,17 +3679,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="634523592"/>
+        <c:crossAx val="2136706712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3324,8 +3704,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3348,7 +3737,9 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -3386,15 +3777,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3406,8 +3807,17 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3425,11 +3835,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -3502,17 +3915,26 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="634998040"/>
-        <c:axId val="635009336"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2128130136"/>
+        <c:axId val="-2128124568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="634998040"/>
+        <c:axId val="-2128130136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -3530,19 +3952,23 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="635009336"/>
+        <c:crossAx val="-2128124568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="635009336"/>
+        <c:axId val="-2128124568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -3561,16 +3987,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="634998040"/>
+        <c:crossAx val="-2128130136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3582,8 +4012,17 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -3623,15 +4062,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3643,8 +4092,17 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3662,15 +4120,19 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'30-Apps'!$A$138:$A$145</c:f>
@@ -3737,39 +4199,55 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="635062952"/>
-        <c:axId val="635053912"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2128073768"/>
+        <c:axId val="-2128070792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="635062952"/>
+        <c:axId val="-2128073768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="635053912"/>
+        <c:crossAx val="-2128070792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="635053912"/>
+        <c:axId val="-2128070792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="635062952"/>
+        <c:crossAx val="-2128073768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3781,9 +4259,19 @@
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -3821,15 +4309,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3841,9 +4339,19 @@
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -3881,15 +4389,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3901,8 +4419,17 @@
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3920,11 +4447,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -4057,18 +4587,27 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="635140200"/>
-        <c:axId val="635147816"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2127996696"/>
+        <c:axId val="-2127991128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="635140200"/>
+        <c:axId val="-2127996696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32.0"/>
           <c:min val="0.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -4086,19 +4625,23 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="635147816"/>
+        <c:crossAx val="-2127991128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="635147816"/>
+        <c:axId val="-2127991128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -4117,16 +4660,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="635140200"/>
+        <c:crossAx val="-2127996696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4140,7 +4687,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr published="0"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="128" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -4705,7 +5252,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8570280" cy="5826014"/>
+    <xdr:ext cx="8572500" cy="5834063"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -5084,7 +5631,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C251"/>
   <sheetViews>
@@ -5092,7 +5639,7 @@
       <selection activeCell="A163" sqref="A163:A165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1">
@@ -6478,7 +7025,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -6486,7 +7033,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C194"/>
   <sheetViews>
@@ -6494,7 +7041,7 @@
       <selection activeCell="C193" sqref="C193"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1">
@@ -7451,14 +7998,13 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A175:B193">
     <sortCondition ref="A175:A193"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -7466,7 +8012,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -7474,7 +8020,7 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -7664,7 +8210,7 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -7672,7 +8218,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -7680,7 +8226,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -7871,7 +8417,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -7879,7 +8425,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -7887,7 +8433,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
   </cols>
@@ -7985,11 +8531,10 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -7997,7 +8542,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J104"/>
   <sheetViews>
@@ -8005,7 +8550,7 @@
       <selection activeCell="J85" sqref="J85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -9192,11 +9737,11 @@
       </c>
       <c r="I83">
         <f>C104*2</f>
-        <v>6.3556544457941193</v>
+        <v>6.3556544457941895</v>
       </c>
       <c r="J83">
         <f>C104*2</f>
-        <v>6.3556544457941193</v>
+        <v>6.3556544457941895</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -9221,11 +9766,11 @@
       </c>
       <c r="I84">
         <f>D104*2</f>
-        <v>7.5309730815848157</v>
+        <v>7.5309730815848477</v>
       </c>
       <c r="J84">
         <f>D104*2</f>
-        <v>7.5309730815848157</v>
+        <v>7.5309730815848477</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -9495,20 +10040,83 @@
       </c>
       <c r="C104">
         <f>STDEV(C2:C101)*1000</f>
-        <v>3.1778272228970597</v>
+        <v>3.1778272228970947</v>
       </c>
       <c r="D104">
         <f>STDEV(D2:D101)*1000</f>
-        <v>3.7654865407924079</v>
+        <v>3.7654865407924238</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="27.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2">
+        <v>41953</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
added txn support to watchtower; added history trimming to bm-data-svc
</commit_message>
<xml_diff>
--- a/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
+++ b/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="65">
   <si>
     <t>Total loops</t>
   </si>
@@ -204,6 +204,24 @@
   <si>
     <t>44ms/1123</t>
   </si>
+  <si>
+    <t>AppEngineMapper#addComment</t>
+  </si>
+  <si>
+    <t>45ms/1233</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Q/C</t>
+  </si>
+  <si>
+    <t>0.95/0.05</t>
+  </si>
+  <si>
+    <t>Nodes</t>
+  </si>
 </sst>
 </file>
 
@@ -531,11 +549,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2128263304"/>
-        <c:axId val="-2128257896"/>
+        <c:axId val="-2123065416"/>
+        <c:axId val="-2123059960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2128263304"/>
+        <c:axId val="-2123065416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,12 +582,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128257896"/>
+        <c:crossAx val="-2123059960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2128257896"/>
+        <c:axId val="-2123059960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -600,7 +618,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128263304"/>
+        <c:crossAx val="-2123065416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -941,11 +959,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2127959960"/>
-        <c:axId val="-2127954152"/>
+        <c:axId val="-2122807704"/>
+        <c:axId val="-2122802008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2127959960"/>
+        <c:axId val="-2122807704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -979,12 +997,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127954152"/>
+        <c:crossAx val="-2122802008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2127954152"/>
+        <c:axId val="-2122802008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1014,7 +1032,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127959960"/>
+        <c:crossAx val="-2122807704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1542,11 +1560,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2129990696"/>
-        <c:axId val="-2129987704"/>
+        <c:axId val="-2122752968"/>
+        <c:axId val="-2122749976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2129990696"/>
+        <c:axId val="-2122752968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1556,12 +1574,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129987704"/>
+        <c:crossAx val="-2122749976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2129987704"/>
+        <c:axId val="-2122749976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1573,7 +1591,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129990696"/>
+        <c:crossAx val="-2122752968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1871,11 +1889,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2129958600"/>
-        <c:axId val="-2129955608"/>
+        <c:axId val="-2122723000"/>
+        <c:axId val="-2122720040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2129958600"/>
+        <c:axId val="-2122723000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1886,12 +1904,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129955608"/>
+        <c:crossAx val="-2122720040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2129955608"/>
+        <c:axId val="-2122720040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1903,7 +1921,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129958600"/>
+        <c:crossAx val="-2122723000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2263,11 +2281,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2129877128"/>
-        <c:axId val="-2129874152"/>
+        <c:axId val="-2122644024"/>
+        <c:axId val="-2122641016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2129877128"/>
+        <c:axId val="-2122644024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2276,7 +2294,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129874152"/>
+        <c:crossAx val="-2122641016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2284,7 +2302,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129874152"/>
+        <c:axId val="-2122641016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2295,7 +2313,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129877128"/>
+        <c:crossAx val="-2122644024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2443,11 +2461,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2129846472"/>
-        <c:axId val="-2129843480"/>
+        <c:axId val="-2122615368"/>
+        <c:axId val="-2122612408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2129846472"/>
+        <c:axId val="-2122615368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -2458,12 +2476,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129843480"/>
+        <c:crossAx val="-2122612408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2129843480"/>
+        <c:axId val="-2122612408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2475,7 +2493,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129846472"/>
+        <c:crossAx val="-2122615368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2763,11 +2781,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2129793128"/>
-        <c:axId val="-2129790136"/>
+        <c:axId val="-2122563832"/>
+        <c:axId val="-2122560872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2129793128"/>
+        <c:axId val="-2122563832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2777,12 +2795,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129790136"/>
+        <c:crossAx val="-2122560872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2129790136"/>
+        <c:axId val="-2122560872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2794,7 +2812,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129793128"/>
+        <c:crossAx val="-2122563832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2846,7 +2864,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2992,11 +3009,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2129740424"/>
-        <c:axId val="-2129737416"/>
+        <c:axId val="-2122510792"/>
+        <c:axId val="-2122507784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2129740424"/>
+        <c:axId val="-2122510792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3015,7 +3032,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2129737416"/>
+        <c:crossAx val="-2122507784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3023,7 +3040,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129737416"/>
+        <c:axId val="-2122507784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3046,7 +3063,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3063,7 +3079,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2129740424"/>
+        <c:crossAx val="-2122510792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3314,11 +3330,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2128189640"/>
-        <c:axId val="-2128184120"/>
+        <c:axId val="-2123030376"/>
+        <c:axId val="-2123024920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2128189640"/>
+        <c:axId val="-2123030376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3347,12 +3363,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128184120"/>
+        <c:crossAx val="-2123024920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2128184120"/>
+        <c:axId val="-2123024920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3382,7 +3398,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128189640"/>
+        <c:crossAx val="-2123030376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3635,11 +3651,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2136706712"/>
-        <c:axId val="2136709688"/>
+        <c:axId val="-2122462184"/>
+        <c:axId val="-2122459208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2136706712"/>
+        <c:axId val="-2122462184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3648,7 +3664,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2136709688"/>
+        <c:crossAx val="-2122459208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3656,7 +3672,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2136709688"/>
+        <c:axId val="-2122459208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3685,7 +3701,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2136706712"/>
+        <c:crossAx val="-2122462184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3925,11 +3941,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2128130136"/>
-        <c:axId val="-2128124568"/>
+        <c:axId val="-2122972536"/>
+        <c:axId val="-2122967048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2128130136"/>
+        <c:axId val="-2122972536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -3958,12 +3974,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128124568"/>
+        <c:crossAx val="-2122967048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2128124568"/>
+        <c:axId val="-2122967048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3993,7 +4009,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128130136"/>
+        <c:crossAx val="-2122972536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4208,11 +4224,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2128073768"/>
-        <c:axId val="-2128070792"/>
+        <c:axId val="-2122917912"/>
+        <c:axId val="-2122914968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2128073768"/>
+        <c:axId val="-2122917912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4221,7 +4237,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128070792"/>
+        <c:crossAx val="-2122914968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4229,7 +4245,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2128070792"/>
+        <c:axId val="-2122914968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4240,7 +4256,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128073768"/>
+        <c:crossAx val="-2122917912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4597,11 +4613,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2127996696"/>
-        <c:axId val="-2127991128"/>
+        <c:axId val="-2122842360"/>
+        <c:axId val="-2122836872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2127996696"/>
+        <c:axId val="-2122842360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32.0"/>
@@ -4631,12 +4647,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127991128"/>
+        <c:crossAx val="-2122836872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2127991128"/>
+        <c:axId val="-2122836872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4666,7 +4682,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127996696"/>
+        <c:crossAx val="-2122842360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10061,23 +10077,42 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="2">
+      <c r="A1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="2">
         <v>41953</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -10111,6 +10146,25 @@
       </c>
       <c r="D6" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10">
+        <v>42</v>
+      </c>
+      <c r="C10">
+        <v>44</v>
+      </c>
+      <c r="D10">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding latest test results
</commit_message>
<xml_diff>
--- a/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
+++ b/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="69">
   <si>
     <t>Total loops</t>
   </si>
@@ -190,25 +190,7 @@
     <t>Actual Quantile (QBETS)</t>
   </si>
   <si>
-    <t>51ms/1123</t>
-  </si>
-  <si>
-    <t>41ms/100</t>
-  </si>
-  <si>
-    <t>44ms/100</t>
-  </si>
-  <si>
-    <t>43ms/1123</t>
-  </si>
-  <si>
-    <t>44ms/1123</t>
-  </si>
-  <si>
     <t>AppEngineMapper#addComment</t>
-  </si>
-  <si>
-    <t>45ms/1233</t>
   </si>
   <si>
     <t>Date</t>
@@ -221,6 +203,36 @@
   </si>
   <si>
     <t>Nodes</t>
+  </si>
+  <si>
+    <t>45ms/1168</t>
+  </si>
+  <si>
+    <t>38ms/100</t>
+  </si>
+  <si>
+    <t>33ms/100</t>
+  </si>
+  <si>
+    <t>34ms/1000</t>
+  </si>
+  <si>
+    <t>35ms/1000</t>
+  </si>
+  <si>
+    <t>43ms/1210</t>
+  </si>
+  <si>
+    <t>43ms/100</t>
+  </si>
+  <si>
+    <t>62ms/100</t>
+  </si>
+  <si>
+    <t>45ms/1000</t>
+  </si>
+  <si>
+    <t>46ms/1000</t>
   </si>
 </sst>
 </file>
@@ -264,12 +276,18 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -290,10 +308,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -344,7 +364,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -549,11 +568,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2123065416"/>
-        <c:axId val="-2123059960"/>
+        <c:axId val="-2124933032"/>
+        <c:axId val="-2125033352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2123065416"/>
+        <c:axId val="-2124933032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -575,19 +594,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123059960"/>
+        <c:crossAx val="-2125033352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2123059960"/>
+        <c:axId val="-2125033352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -611,14 +629,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123065416"/>
+        <c:crossAx val="-2124933032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -959,11 +976,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2122807704"/>
-        <c:axId val="-2122802008"/>
+        <c:axId val="-2122427208"/>
+        <c:axId val="-2122421512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2122807704"/>
+        <c:axId val="-2122427208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -997,12 +1014,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122802008"/>
+        <c:crossAx val="-2122421512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2122802008"/>
+        <c:axId val="-2122421512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1032,7 +1049,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122807704"/>
+        <c:crossAx val="-2122427208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1560,11 +1577,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2122752968"/>
-        <c:axId val="-2122749976"/>
+        <c:axId val="-2130438440"/>
+        <c:axId val="-2130473560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2122752968"/>
+        <c:axId val="-2130438440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1574,12 +1591,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122749976"/>
+        <c:crossAx val="-2130473560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2122749976"/>
+        <c:axId val="-2130473560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1591,7 +1608,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122752968"/>
+        <c:crossAx val="-2130438440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1889,11 +1906,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2122723000"/>
-        <c:axId val="-2122720040"/>
+        <c:axId val="-2129695928"/>
+        <c:axId val="-2130617128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2122723000"/>
+        <c:axId val="-2129695928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1904,12 +1921,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122720040"/>
+        <c:crossAx val="-2130617128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2122720040"/>
+        <c:axId val="-2130617128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1921,7 +1938,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122723000"/>
+        <c:crossAx val="-2129695928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2281,11 +2298,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2122644024"/>
-        <c:axId val="-2122641016"/>
+        <c:axId val="-2130628312"/>
+        <c:axId val="-2129947096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2122644024"/>
+        <c:axId val="-2130628312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2294,7 +2311,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122641016"/>
+        <c:crossAx val="-2129947096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2302,7 +2319,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122641016"/>
+        <c:axId val="-2129947096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2313,7 +2330,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122644024"/>
+        <c:crossAx val="-2130628312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2461,11 +2478,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2122615368"/>
-        <c:axId val="-2122612408"/>
+        <c:axId val="-2129756056"/>
+        <c:axId val="2093796376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2122615368"/>
+        <c:axId val="-2129756056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -2476,12 +2493,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122612408"/>
+        <c:crossAx val="2093796376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2122612408"/>
+        <c:axId val="2093796376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2493,7 +2510,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122615368"/>
+        <c:crossAx val="-2129756056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2781,11 +2798,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2122563832"/>
-        <c:axId val="-2122560872"/>
+        <c:axId val="-2124089496"/>
+        <c:axId val="-2124086488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2122563832"/>
+        <c:axId val="-2124089496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2795,12 +2812,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122560872"/>
+        <c:crossAx val="-2124086488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2122560872"/>
+        <c:axId val="-2124086488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2812,7 +2829,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122563832"/>
+        <c:crossAx val="-2124089496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3009,11 +3026,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2122510792"/>
-        <c:axId val="-2122507784"/>
+        <c:axId val="-2125779096"/>
+        <c:axId val="2028123304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2122510792"/>
+        <c:axId val="-2125779096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3032,7 +3049,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122507784"/>
+        <c:crossAx val="2028123304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3040,7 +3057,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122507784"/>
+        <c:axId val="2028123304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3079,7 +3096,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122510792"/>
+        <c:crossAx val="-2125779096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3330,11 +3347,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2123030376"/>
-        <c:axId val="-2123024920"/>
+        <c:axId val="-2123627624"/>
+        <c:axId val="-2124128968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2123030376"/>
+        <c:axId val="-2123627624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3363,12 +3380,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123024920"/>
+        <c:crossAx val="-2124128968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2123024920"/>
+        <c:axId val="-2124128968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3398,7 +3415,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123030376"/>
+        <c:crossAx val="-2123627624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3651,11 +3668,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2122462184"/>
-        <c:axId val="-2122459208"/>
+        <c:axId val="-2123711352"/>
+        <c:axId val="-2123708376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2122462184"/>
+        <c:axId val="-2123711352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3664,7 +3681,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122459208"/>
+        <c:crossAx val="-2123708376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3672,7 +3689,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122459208"/>
+        <c:axId val="-2123708376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3701,7 +3718,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122462184"/>
+        <c:crossAx val="-2123711352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3941,11 +3958,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2122972536"/>
-        <c:axId val="-2122967048"/>
+        <c:axId val="-2124198008"/>
+        <c:axId val="-2124192792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2122972536"/>
+        <c:axId val="-2124198008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -3974,12 +3991,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122967048"/>
+        <c:crossAx val="-2124192792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2122967048"/>
+        <c:axId val="-2124192792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4009,7 +4026,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122972536"/>
+        <c:crossAx val="-2124198008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4224,11 +4241,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2122917912"/>
-        <c:axId val="-2122914968"/>
+        <c:axId val="-2123787496"/>
+        <c:axId val="-2123861752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2122917912"/>
+        <c:axId val="-2123787496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4237,7 +4254,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122914968"/>
+        <c:crossAx val="-2123861752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4245,7 +4262,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122914968"/>
+        <c:axId val="-2123861752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4256,7 +4273,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122917912"/>
+        <c:crossAx val="-2123787496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4613,11 +4630,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2122842360"/>
-        <c:axId val="-2122836872"/>
+        <c:axId val="-2122569464"/>
+        <c:axId val="-2122668664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2122842360"/>
+        <c:axId val="-2122569464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32.0"/>
@@ -4647,12 +4664,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122836872"/>
+        <c:crossAx val="-2122668664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2122836872"/>
+        <c:axId val="-2122668664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4682,7 +4699,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122842360"/>
+        <c:crossAx val="-2122569464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10079,7 +10096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -10093,78 +10110,85 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="2">
+        <v>41954</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="2">
-        <v>41953</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="C7" t="s">
         <v>62</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
         <v>64</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="C6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" t="s">
-        <v>60</v>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="B10">
-        <v>42</v>
-      </c>
-      <c r="C10">
-        <v>44</v>
-      </c>
-      <c r="D10">
-        <v>46</v>
+      <c r="C10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
better error handling for kitty
</commit_message>
<xml_diff>
--- a/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
+++ b/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
   <si>
     <t>Total loops</t>
   </si>
@@ -234,6 +234,18 @@
   <si>
     <t>46ms/1000</t>
   </si>
+  <si>
+    <t>SimpleRestApp#put</t>
+  </si>
+  <si>
+    <t>42ms/2792</t>
+  </si>
+  <si>
+    <t>50ms/1000</t>
+  </si>
+  <si>
+    <t>49ms/1000</t>
+  </si>
 </sst>
 </file>
 
@@ -568,11 +580,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2124933032"/>
-        <c:axId val="-2125033352"/>
+        <c:axId val="-2130456296"/>
+        <c:axId val="-2129677208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2124933032"/>
+        <c:axId val="-2130456296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -600,12 +612,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2125033352"/>
+        <c:crossAx val="-2129677208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2125033352"/>
+        <c:axId val="-2129677208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -635,7 +647,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124933032"/>
+        <c:crossAx val="-2130456296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -976,11 +988,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2122427208"/>
-        <c:axId val="-2122421512"/>
+        <c:axId val="-2125260520"/>
+        <c:axId val="-2125266216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2122427208"/>
+        <c:axId val="-2125260520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1014,12 +1026,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122421512"/>
+        <c:crossAx val="-2125266216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2122421512"/>
+        <c:axId val="-2125266216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1049,7 +1061,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122427208"/>
+        <c:crossAx val="-2125260520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1577,11 +1589,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2130438440"/>
-        <c:axId val="-2130473560"/>
+        <c:axId val="-2125315384"/>
+        <c:axId val="-2125318376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2130438440"/>
+        <c:axId val="-2125315384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1591,12 +1603,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130473560"/>
+        <c:crossAx val="-2125318376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2130473560"/>
+        <c:axId val="-2125318376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1608,7 +1620,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130438440"/>
+        <c:crossAx val="-2125315384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1906,11 +1918,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2129695928"/>
-        <c:axId val="-2130617128"/>
+        <c:axId val="-2125345544"/>
+        <c:axId val="-2125348504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2129695928"/>
+        <c:axId val="-2125345544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1921,12 +1933,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130617128"/>
+        <c:crossAx val="-2125348504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2130617128"/>
+        <c:axId val="-2125348504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1938,7 +1950,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129695928"/>
+        <c:crossAx val="-2125345544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2298,11 +2310,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2130628312"/>
-        <c:axId val="-2129947096"/>
+        <c:axId val="-2125425032"/>
+        <c:axId val="-2125428056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130628312"/>
+        <c:axId val="-2125425032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2311,7 +2323,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129947096"/>
+        <c:crossAx val="-2125428056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2319,7 +2331,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129947096"/>
+        <c:axId val="-2125428056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2330,7 +2342,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130628312"/>
+        <c:crossAx val="-2125425032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2478,11 +2490,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2129756056"/>
-        <c:axId val="2093796376"/>
+        <c:axId val="-2125453880"/>
+        <c:axId val="-2125456840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2129756056"/>
+        <c:axId val="-2125453880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -2493,12 +2505,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2093796376"/>
+        <c:crossAx val="-2125456840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2093796376"/>
+        <c:axId val="-2125456840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2510,7 +2522,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129756056"/>
+        <c:crossAx val="-2125453880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2798,11 +2810,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2124089496"/>
-        <c:axId val="-2124086488"/>
+        <c:axId val="-2128777160"/>
+        <c:axId val="-2128862808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2124089496"/>
+        <c:axId val="-2128777160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2812,12 +2824,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124086488"/>
+        <c:crossAx val="-2128862808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2124086488"/>
+        <c:axId val="-2128862808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2829,7 +2841,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124089496"/>
+        <c:crossAx val="-2128777160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3026,11 +3038,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2125779096"/>
-        <c:axId val="2028123304"/>
+        <c:axId val="-2129009176"/>
+        <c:axId val="2094982472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2125779096"/>
+        <c:axId val="-2129009176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3049,7 +3061,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2028123304"/>
+        <c:crossAx val="2094982472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3057,7 +3069,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2028123304"/>
+        <c:axId val="2094982472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3096,7 +3108,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125779096"/>
+        <c:crossAx val="-2129009176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3347,11 +3359,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2123627624"/>
-        <c:axId val="-2124128968"/>
+        <c:axId val="-2124900552"/>
+        <c:axId val="-2130438824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2123627624"/>
+        <c:axId val="-2124900552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3380,12 +3392,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124128968"/>
+        <c:crossAx val="-2130438824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2124128968"/>
+        <c:axId val="-2130438824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3415,7 +3427,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123627624"/>
+        <c:crossAx val="-2124900552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3462,6 +3474,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3668,11 +3681,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2123711352"/>
-        <c:axId val="-2123708376"/>
+        <c:axId val="-2128863704"/>
+        <c:axId val="-2128781192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2123711352"/>
+        <c:axId val="-2128863704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3681,7 +3694,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123708376"/>
+        <c:crossAx val="-2128781192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3689,7 +3702,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2123708376"/>
+        <c:axId val="-2128781192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3712,13 +3725,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123711352"/>
+        <c:crossAx val="-2128863704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3958,11 +3972,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2124198008"/>
-        <c:axId val="-2124192792"/>
+        <c:axId val="-2124534760"/>
+        <c:axId val="-2124529272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2124198008"/>
+        <c:axId val="-2124534760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -3991,12 +4005,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124192792"/>
+        <c:crossAx val="-2124529272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2124192792"/>
+        <c:axId val="-2124529272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4026,7 +4040,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124198008"/>
+        <c:crossAx val="-2124534760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4241,11 +4255,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2123787496"/>
-        <c:axId val="-2123861752"/>
+        <c:axId val="-2124480136"/>
+        <c:axId val="-2124477192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2123787496"/>
+        <c:axId val="-2124480136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4254,7 +4268,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123861752"/>
+        <c:crossAx val="-2124477192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4262,7 +4276,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2123861752"/>
+        <c:axId val="-2124477192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4273,7 +4287,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123787496"/>
+        <c:crossAx val="-2124480136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4630,11 +4644,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2122569464"/>
-        <c:axId val="-2122668664"/>
+        <c:axId val="-2125225880"/>
+        <c:axId val="-2125231368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2122569464"/>
+        <c:axId val="-2125225880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32.0"/>
@@ -4664,12 +4678,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122668664"/>
+        <c:crossAx val="-2125231368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2122668664"/>
+        <c:axId val="-2125231368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4699,7 +4713,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122569464"/>
+        <c:crossAx val="-2125225880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8468,7 +8482,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -10094,10 +10108,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10191,6 +10205,20 @@
         <v>68</v>
       </c>
     </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
second round test results
</commit_message>
<xml_diff>
--- a/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
+++ b/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16380" tabRatio="500" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="30-Apps" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
   <si>
     <t>Total loops</t>
   </si>
@@ -249,6 +249,30 @@
   <si>
     <t>SimpleRestApp#get</t>
   </si>
+  <si>
+    <t>60ms/1183</t>
+  </si>
+  <si>
+    <t>42ms/1000</t>
+  </si>
+  <si>
+    <t>53ms/1183</t>
+  </si>
+  <si>
+    <t>57ms/1000</t>
+  </si>
+  <si>
+    <t>59ms/1000</t>
+  </si>
+  <si>
+    <t>16ms/1183</t>
+  </si>
+  <si>
+    <t>53ms/1000</t>
+  </si>
+  <si>
+    <t>7ms/1000</t>
+  </si>
 </sst>
 </file>
 
@@ -291,7 +315,7 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,6 +325,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -314,7 +344,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -322,21 +352,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -583,11 +625,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2127836840"/>
-        <c:axId val="-2127831384"/>
+        <c:axId val="-2124637832"/>
+        <c:axId val="-2129549032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2127836840"/>
+        <c:axId val="-2124637832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -615,12 +657,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127831384"/>
+        <c:crossAx val="-2129549032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2127831384"/>
+        <c:axId val="-2129549032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -650,7 +692,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127836840"/>
+        <c:crossAx val="-2124637832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -991,11 +1033,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2111181992"/>
-        <c:axId val="-2111552024"/>
+        <c:axId val="-2122851944"/>
+        <c:axId val="-2127938168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2111181992"/>
+        <c:axId val="-2122851944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1029,12 +1071,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111552024"/>
+        <c:crossAx val="-2127938168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2111552024"/>
+        <c:axId val="-2127938168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1064,7 +1106,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111181992"/>
+        <c:crossAx val="-2122851944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1592,11 +1634,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2111077144"/>
-        <c:axId val="-2111574328"/>
+        <c:axId val="-2124970232"/>
+        <c:axId val="-2129741656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2111077144"/>
+        <c:axId val="-2124970232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1606,12 +1648,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111574328"/>
+        <c:crossAx val="-2129741656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2111574328"/>
+        <c:axId val="-2129741656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1623,7 +1665,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111077144"/>
+        <c:crossAx val="-2124970232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1921,11 +1963,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2111250264"/>
-        <c:axId val="2094986504"/>
+        <c:axId val="-2124486936"/>
+        <c:axId val="-2124483976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2111250264"/>
+        <c:axId val="-2124486936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1936,12 +1978,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2094986504"/>
+        <c:crossAx val="-2124483976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2094986504"/>
+        <c:axId val="-2124483976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1953,7 +1995,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111250264"/>
+        <c:crossAx val="-2124486936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2313,11 +2355,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2111460728"/>
-        <c:axId val="-2111499096"/>
+        <c:axId val="-2124968456"/>
+        <c:axId val="-2124577432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2111460728"/>
+        <c:axId val="-2124968456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2326,7 +2368,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111499096"/>
+        <c:crossAx val="-2124577432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2334,7 +2376,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2111499096"/>
+        <c:axId val="-2124577432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2345,7 +2387,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111460728"/>
+        <c:crossAx val="-2124968456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2493,11 +2535,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2111456392"/>
-        <c:axId val="-2111453432"/>
+        <c:axId val="-2125212120"/>
+        <c:axId val="-2125209160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2111456392"/>
+        <c:axId val="-2125212120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -2508,12 +2550,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111453432"/>
+        <c:crossAx val="-2125209160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2111453432"/>
+        <c:axId val="-2125209160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2525,7 +2567,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111456392"/>
+        <c:crossAx val="-2125212120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2813,11 +2855,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2111294344"/>
-        <c:axId val="-2111291384"/>
+        <c:axId val="-2129994520"/>
+        <c:axId val="-2125425240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2111294344"/>
+        <c:axId val="-2129994520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2827,12 +2869,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111291384"/>
+        <c:crossAx val="-2125425240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2111291384"/>
+        <c:axId val="-2125425240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2844,7 +2886,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111294344"/>
+        <c:crossAx val="-2129994520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3041,11 +3083,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2111132776"/>
-        <c:axId val="-2111128952"/>
+        <c:axId val="-2125375352"/>
+        <c:axId val="-2125372344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2111132776"/>
+        <c:axId val="-2125375352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3064,7 +3106,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2111128952"/>
+        <c:crossAx val="-2125372344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3072,7 +3114,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2111128952"/>
+        <c:axId val="-2125372344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3111,7 +3153,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2111132776"/>
+        <c:crossAx val="-2125375352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3362,11 +3404,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2122996008"/>
-        <c:axId val="-2122598664"/>
+        <c:axId val="-2111054504"/>
+        <c:axId val="-2111422248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2122996008"/>
+        <c:axId val="-2111054504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3395,12 +3437,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122598664"/>
+        <c:crossAx val="-2111422248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2122598664"/>
+        <c:axId val="-2111422248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3430,7 +3472,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122996008"/>
+        <c:crossAx val="-2111054504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3683,11 +3725,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2110939640"/>
-        <c:axId val="-2110935816"/>
+        <c:axId val="-2111073448"/>
+        <c:axId val="-2111070472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2110939640"/>
+        <c:axId val="-2111073448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3696,7 +3738,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110935816"/>
+        <c:crossAx val="-2111070472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3704,7 +3746,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2110935816"/>
+        <c:axId val="-2111070472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3733,7 +3775,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110939640"/>
+        <c:crossAx val="-2111073448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3973,11 +4015,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2128032840"/>
-        <c:axId val="-2128036488"/>
+        <c:axId val="-2126081704"/>
+        <c:axId val="-2126082104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2128032840"/>
+        <c:axId val="-2126081704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -4006,12 +4048,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128036488"/>
+        <c:crossAx val="-2126082104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2128036488"/>
+        <c:axId val="-2126082104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4041,7 +4083,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128032840"/>
+        <c:crossAx val="-2126081704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4256,11 +4298,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2128089592"/>
-        <c:axId val="-2128094216"/>
+        <c:axId val="2136406376"/>
+        <c:axId val="-2122505624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2128089592"/>
+        <c:axId val="2136406376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4269,7 +4311,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128094216"/>
+        <c:crossAx val="-2122505624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4277,7 +4319,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2128094216"/>
+        <c:axId val="-2122505624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4288,7 +4330,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128089592"/>
+        <c:crossAx val="2136406376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4645,11 +4687,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2111479224"/>
-        <c:axId val="-2111354040"/>
+        <c:axId val="-2122564280"/>
+        <c:axId val="-2122916280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2111479224"/>
+        <c:axId val="-2122564280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32.0"/>
@@ -4679,12 +4721,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111354040"/>
+        <c:crossAx val="-2122916280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2111354040"/>
+        <c:axId val="-2122916280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4714,7 +4756,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111479224"/>
+        <c:crossAx val="-2122564280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10109,10 +10151,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10121,108 +10163,201 @@
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B1" s="2">
         <v>41954</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="6">
+        <v>41959</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:4">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="1:8">
+      <c r="B5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="F5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>44</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="C7" t="s">
+      <c r="F6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>54</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" t="s">
+      <c r="F9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>69</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="F12" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>73</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="F13" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added custom time series predictor to the bm service
</commit_message>
<xml_diff>
--- a/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
+++ b/Eager/eager-static-analyzer/results/StaticAnalysisResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16380" tabRatio="500" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16080" tabRatio="500" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="30-Apps" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="84">
   <si>
     <t>Total loops</t>
   </si>
@@ -262,16 +262,22 @@
     <t>57ms/1000</t>
   </si>
   <si>
-    <t>59ms/1000</t>
-  </si>
-  <si>
     <t>16ms/1183</t>
   </si>
   <si>
-    <t>53ms/1000</t>
+    <t>19ms/1000</t>
   </si>
   <si>
-    <t>7ms/1000</t>
+    <t>56ms/1000</t>
+  </si>
+  <si>
+    <t>Application#Operation</t>
+  </si>
+  <si>
+    <t>52ms/1000</t>
+  </si>
+  <si>
+    <t>51ms/1000</t>
   </si>
 </sst>
 </file>
@@ -625,11 +631,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2124637832"/>
-        <c:axId val="-2129549032"/>
+        <c:axId val="-2128140152"/>
+        <c:axId val="-2128134872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2124637832"/>
+        <c:axId val="-2128140152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,12 +663,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129549032"/>
+        <c:crossAx val="-2128134872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2129549032"/>
+        <c:axId val="-2128134872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -692,7 +698,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124637832"/>
+        <c:crossAx val="-2128140152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1033,11 +1039,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2122851944"/>
-        <c:axId val="-2127938168"/>
+        <c:axId val="-2127951416"/>
+        <c:axId val="-2123324088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2122851944"/>
+        <c:axId val="-2127951416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1071,12 +1077,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127938168"/>
+        <c:crossAx val="-2123324088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2127938168"/>
+        <c:axId val="-2123324088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1106,7 +1112,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122851944"/>
+        <c:crossAx val="-2127951416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1634,11 +1640,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2124970232"/>
-        <c:axId val="-2129741656"/>
+        <c:axId val="-2127922728"/>
+        <c:axId val="-2123070952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2124970232"/>
+        <c:axId val="-2127922728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1648,12 +1654,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129741656"/>
+        <c:crossAx val="-2123070952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2129741656"/>
+        <c:axId val="-2123070952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1665,7 +1671,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124970232"/>
+        <c:crossAx val="-2127922728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1963,11 +1969,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2124486936"/>
-        <c:axId val="-2124483976"/>
+        <c:axId val="-2122601608"/>
+        <c:axId val="-2127992424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2124486936"/>
+        <c:axId val="-2122601608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1978,12 +1984,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124483976"/>
+        <c:crossAx val="-2127992424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2124483976"/>
+        <c:axId val="-2127992424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1995,7 +2001,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124486936"/>
+        <c:crossAx val="-2122601608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2355,11 +2361,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2124968456"/>
-        <c:axId val="-2124577432"/>
+        <c:axId val="-2127733224"/>
+        <c:axId val="-2127730440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2124968456"/>
+        <c:axId val="-2127733224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2368,7 +2374,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124577432"/>
+        <c:crossAx val="-2127730440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2376,7 +2382,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124577432"/>
+        <c:axId val="-2127730440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2387,7 +2393,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124968456"/>
+        <c:crossAx val="-2127733224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2535,11 +2541,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2125212120"/>
-        <c:axId val="-2125209160"/>
+        <c:axId val="-2122425416"/>
+        <c:axId val="-2127886328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2125212120"/>
+        <c:axId val="-2122425416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -2550,12 +2556,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2125209160"/>
+        <c:crossAx val="-2127886328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2125209160"/>
+        <c:axId val="-2127886328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2567,7 +2573,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2125212120"/>
+        <c:crossAx val="-2122425416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2855,11 +2861,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2129994520"/>
-        <c:axId val="-2125425240"/>
+        <c:axId val="-2128020520"/>
+        <c:axId val="-2122508248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2129994520"/>
+        <c:axId val="-2128020520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2869,12 +2875,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2125425240"/>
+        <c:crossAx val="-2122508248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2125425240"/>
+        <c:axId val="-2122508248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2886,7 +2892,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129994520"/>
+        <c:crossAx val="-2128020520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3083,11 +3089,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2125375352"/>
-        <c:axId val="-2125372344"/>
+        <c:axId val="-2128201640"/>
+        <c:axId val="-2128198664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2125375352"/>
+        <c:axId val="-2128201640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3106,7 +3112,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125372344"/>
+        <c:crossAx val="-2128198664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3114,7 +3120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2125372344"/>
+        <c:axId val="-2128198664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3153,7 +3159,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125375352"/>
+        <c:crossAx val="-2128201640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3404,11 +3410,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2111054504"/>
-        <c:axId val="-2111422248"/>
+        <c:axId val="-2122418488"/>
+        <c:axId val="-2123345224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2111054504"/>
+        <c:axId val="-2122418488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3437,12 +3443,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111422248"/>
+        <c:crossAx val="-2123345224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2111422248"/>
+        <c:axId val="-2123345224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3472,7 +3478,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111054504"/>
+        <c:crossAx val="-2122418488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3725,11 +3731,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2111073448"/>
-        <c:axId val="-2111070472"/>
+        <c:axId val="-2128286184"/>
+        <c:axId val="-2128299880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2111073448"/>
+        <c:axId val="-2128286184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3738,7 +3744,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111070472"/>
+        <c:crossAx val="-2128299880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3746,7 +3752,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2111070472"/>
+        <c:axId val="-2128299880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3775,11 +3781,272 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111073448"/>
+        <c:crossAx val="-2128286184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparison of Predicted and Actual Quantiles</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Kitty!$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Prediction (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Kitty!$A$17:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>ServerHealth#info</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AppEngineMapper#addComment</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SimpleRestApp#put</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SimpleRestApp#get</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Kitty!$B$17:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Kitty!$C$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Kitty!$A$17:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>ServerHealth#info</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AppEngineMapper#addComment</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SimpleRestApp#put</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SimpleRestApp#get</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Kitty!$C$17:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2123644264"/>
+        <c:axId val="-2122685480"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2123644264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>App#Op</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2122685480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2122685480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="60.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>0.95</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Quantile of Execution Time (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2123644264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4015,11 +4282,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2126081704"/>
-        <c:axId val="-2126082104"/>
+        <c:axId val="-2122438600"/>
+        <c:axId val="-2128104712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2126081704"/>
+        <c:axId val="-2122438600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -4048,12 +4315,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126082104"/>
+        <c:crossAx val="-2128104712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2126082104"/>
+        <c:axId val="-2128104712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4083,7 +4350,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126081704"/>
+        <c:crossAx val="-2122438600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4298,11 +4565,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2136406376"/>
-        <c:axId val="-2122505624"/>
+        <c:axId val="-2128114168"/>
+        <c:axId val="-2127902488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2136406376"/>
+        <c:axId val="-2128114168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4311,7 +4578,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122505624"/>
+        <c:crossAx val="-2127902488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4319,7 +4586,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122505624"/>
+        <c:axId val="-2127902488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4330,7 +4597,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2136406376"/>
+        <c:crossAx val="-2128114168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4687,11 +4954,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2122564280"/>
-        <c:axId val="-2122916280"/>
+        <c:axId val="-2123027176"/>
+        <c:axId val="-2127804424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2122564280"/>
+        <c:axId val="-2123027176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32.0"/>
@@ -4721,12 +4988,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122916280"/>
+        <c:crossAx val="-2127804424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2122916280"/>
+        <c:axId val="-2127804424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4756,7 +5023,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122564280"/>
+        <c:crossAx val="-2123027176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5400,6 +5667,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1127760</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>187960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>792480</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -10151,10 +10453,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10294,10 +10596,10 @@
         <v>76</v>
       </c>
       <c r="G9" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -10337,10 +10639,10 @@
         <v>76</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -10351,17 +10653,73 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="F13" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="H13" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>81</v>
+      <c r="B16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17">
+        <v>60</v>
+      </c>
+      <c r="C17">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18">
+        <v>53</v>
+      </c>
+      <c r="C18">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19">
+        <v>53</v>
+      </c>
+      <c r="C19">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>